<commit_message>
wip on test iterations
</commit_message>
<xml_diff>
--- a/docs/testResources/MasterTestSuite.xlsx
+++ b/docs/testResources/MasterTestSuite.xlsx
@@ -5,11 +5,11 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Siwapiwe Mbiko\Documents\GitHub\eohmc-selenium-core\src\test\java\eohmc\selenium\core\testResources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\xy40224\Documents\Projects\eohmc-selenium-core\docs\testResources\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20436" windowHeight="7692" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20430" windowHeight="7695" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="OVERVIEW" sheetId="6" r:id="rId1"/>
@@ -1226,6 +1226,21 @@
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="5" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="164" fontId="22" fillId="8" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="22" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="164" fontId="22" fillId="8" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1235,6 +1250,21 @@
     <xf numFmtId="164" fontId="22" fillId="8" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="164" fontId="22" fillId="8" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="16" fontId="20" fillId="9" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="12" fillId="7" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="12" fillId="7" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="164" fontId="22" fillId="8" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1244,44 +1274,95 @@
     <xf numFmtId="164" fontId="22" fillId="8" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="16" fontId="20" fillId="9" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="22" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="16" fontId="20" fillId="9" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="16" fontId="20" fillId="9" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="5" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="5" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="2" fontId="5" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="5" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="3" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="10" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="16" fontId="20" fillId="9" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="10" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="12" fillId="7" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="11" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="12" fillId="7" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="11" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="22" fillId="8" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="22" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="22" fillId="8" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="22" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="3" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="14" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="2" fontId="6" fillId="5" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1289,12 +1370,6 @@
     <xf numFmtId="2" fontId="6" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="3">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
@@ -1302,81 +1377,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="3" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="10" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="10" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="11" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="11" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="3" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="14" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="5" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="5" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="2" fontId="5" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="5" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyFill="1"/>
@@ -2813,11 +2813,11 @@
         </c:dLbls>
         <c:gapWidth val="90"/>
         <c:overlap val="100"/>
-        <c:axId val="-950117984"/>
-        <c:axId val="-950117440"/>
+        <c:axId val="217861744"/>
+        <c:axId val="217862528"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-950117984"/>
+        <c:axId val="217861744"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2860,7 +2860,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-950117440"/>
+        <c:crossAx val="217862528"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2868,7 +2868,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-950117440"/>
+        <c:axId val="217862528"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2919,7 +2919,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-950117984"/>
+        <c:crossAx val="217861744"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="0.5"/>
@@ -3229,8 +3229,8 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="90"/>
-        <c:axId val="-950115808"/>
-        <c:axId val="-950131040"/>
+        <c:axId val="217863312"/>
+        <c:axId val="217863704"/>
       </c:barChart>
       <c:lineChart>
         <c:grouping val="standard"/>
@@ -3420,11 +3420,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-950115808"/>
-        <c:axId val="-950131040"/>
+        <c:axId val="217863312"/>
+        <c:axId val="217863704"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-950115808"/>
+        <c:axId val="217863312"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3467,7 +3467,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-950131040"/>
+        <c:crossAx val="217863704"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3475,7 +3475,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-950131040"/>
+        <c:axId val="217863704"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3538,7 +3538,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-950115808"/>
+        <c:crossAx val="217863312"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -5824,13 +5824,13 @@
       <selection activeCell="B49" sqref="B49"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.2"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" width="9.3984375" style="16" customWidth="1"/>
+    <col min="1" max="1" width="9.375" style="16" customWidth="1"/>
     <col min="2" max="2" width="29.5" style="16" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="34.8984375" style="16" customWidth="1"/>
-    <col min="4" max="4" width="13.59765625" style="16" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="19.19921875" style="16" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="34.875" style="16" customWidth="1"/>
+    <col min="4" max="4" width="13.625" style="16" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.25" style="16" bestFit="1" customWidth="1"/>
     <col min="6" max="16384" width="9" style="16"/>
   </cols>
   <sheetData>
@@ -5856,7 +5856,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="13.8">
+    <row r="4" spans="1:3" ht="14.25">
       <c r="B4" s="24" t="s">
         <v>34</v>
       </c>
@@ -5864,25 +5864,25 @@
         <v>66</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="13.8">
+    <row r="6" spans="1:3" ht="14.25">
       <c r="B6" s="24" t="s">
         <v>33</v>
       </c>
       <c r="C6" s="23"/>
     </row>
-    <row r="7" spans="1:3" ht="13.8">
+    <row r="7" spans="1:3" ht="14.25">
       <c r="B7" s="24" t="s">
         <v>32</v>
       </c>
       <c r="C7" s="23"/>
     </row>
-    <row r="8" spans="1:3" ht="13.8">
+    <row r="8" spans="1:3" ht="14.25">
       <c r="B8" s="24" t="s">
         <v>31</v>
       </c>
       <c r="C8" s="23"/>
     </row>
-    <row r="9" spans="1:3" ht="13.8">
+    <row r="9" spans="1:3" ht="14.25">
       <c r="B9" s="24" t="s">
         <v>30</v>
       </c>
@@ -5909,43 +5909,43 @@
       </c>
       <c r="C15" s="23"/>
     </row>
-    <row r="16" spans="1:3" ht="13.8">
+    <row r="16" spans="1:3" ht="14.25">
       <c r="B16" s="24" t="s">
         <v>27</v>
       </c>
       <c r="C16" s="23"/>
     </row>
-    <row r="17" spans="2:3" ht="13.8">
+    <row r="17" spans="2:3" ht="14.25">
       <c r="B17" s="24" t="s">
         <v>26</v>
       </c>
       <c r="C17" s="23"/>
     </row>
-    <row r="18" spans="2:3" ht="13.8">
+    <row r="18" spans="2:3" ht="14.25">
       <c r="B18" s="24" t="s">
         <v>25</v>
       </c>
       <c r="C18" s="23"/>
     </row>
-    <row r="19" spans="2:3" ht="13.8">
+    <row r="19" spans="2:3" ht="14.25">
       <c r="B19" s="24" t="s">
         <v>24</v>
       </c>
       <c r="C19" s="23"/>
     </row>
-    <row r="20" spans="2:3" ht="13.8">
+    <row r="20" spans="2:3" ht="14.25">
       <c r="B20" s="24" t="s">
         <v>23</v>
       </c>
       <c r="C20" s="23"/>
     </row>
-    <row r="23" spans="2:3" ht="13.8">
+    <row r="23" spans="2:3" ht="15">
       <c r="B23" s="27" t="s">
         <v>50</v>
       </c>
       <c r="C23" s="23"/>
     </row>
-    <row r="25" spans="2:3" ht="13.8">
+    <row r="25" spans="2:3" ht="15">
       <c r="B25" s="25" t="s">
         <v>22</v>
       </c>
@@ -6004,42 +6004,42 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q46"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A10" workbookViewId="0">
       <selection activeCell="G19" sqref="G19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="1" width="12.59765625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.19921875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.25" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="21" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.3984375" customWidth="1"/>
-    <col min="5" max="5" width="25.8984375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.19921875" customWidth="1"/>
+    <col min="4" max="4" width="16.375" customWidth="1"/>
+    <col min="5" max="5" width="25.875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.25" customWidth="1"/>
     <col min="7" max="7" width="13" customWidth="1"/>
-    <col min="8" max="8" width="18.3984375" customWidth="1"/>
-    <col min="9" max="9" width="21.8984375" customWidth="1"/>
-    <col min="10" max="10" width="16.19921875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="18.09765625" customWidth="1"/>
-    <col min="12" max="12" width="22.19921875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="18.375" customWidth="1"/>
+    <col min="9" max="9" width="21.875" customWidth="1"/>
+    <col min="10" max="10" width="16.25" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="18.125" customWidth="1"/>
+    <col min="12" max="12" width="22.25" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="15" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="14.19921875" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="11.19921875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="14.25" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="11.25" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="6.5" customWidth="1"/>
-    <col min="17" max="17" width="11.19921875" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="11.25" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="30" customHeight="1">
-      <c r="A1" s="71" t="s">
+      <c r="A1" s="56" t="s">
         <v>48</v>
       </c>
-      <c r="B1" s="71"/>
-      <c r="C1" s="71"/>
-      <c r="D1" s="71"/>
-      <c r="E1" s="71"/>
-      <c r="F1" s="71"/>
-      <c r="G1" s="71"/>
-      <c r="H1" s="72"/>
+      <c r="B1" s="56"/>
+      <c r="C1" s="56"/>
+      <c r="D1" s="56"/>
+      <c r="E1" s="56"/>
+      <c r="F1" s="56"/>
+      <c r="G1" s="56"/>
+      <c r="H1" s="57"/>
       <c r="I1" s="34" t="s">
         <v>46</v>
       </c>
@@ -6054,16 +6054,16 @@
       </c>
     </row>
     <row r="2" spans="1:17" ht="15" customHeight="1">
-      <c r="A2" s="74" t="s">
+      <c r="A2" s="65" t="s">
         <v>47</v>
       </c>
-      <c r="B2" s="74"/>
-      <c r="C2" s="74"/>
-      <c r="D2" s="74"/>
-      <c r="E2" s="74"/>
-      <c r="F2" s="74"/>
-      <c r="G2" s="74"/>
-      <c r="H2" s="74"/>
+      <c r="B2" s="65"/>
+      <c r="C2" s="65"/>
+      <c r="D2" s="65"/>
+      <c r="E2" s="65"/>
+      <c r="F2" s="65"/>
+      <c r="G2" s="65"/>
+      <c r="H2" s="65"/>
       <c r="I2" s="33" t="s">
         <v>42</v>
       </c>
@@ -6078,14 +6078,14 @@
       </c>
     </row>
     <row r="3" spans="1:17" ht="15" customHeight="1">
-      <c r="A3" s="74"/>
-      <c r="B3" s="74"/>
-      <c r="C3" s="74"/>
-      <c r="D3" s="74"/>
-      <c r="E3" s="74"/>
-      <c r="F3" s="74"/>
-      <c r="G3" s="74"/>
-      <c r="H3" s="74"/>
+      <c r="A3" s="65"/>
+      <c r="B3" s="65"/>
+      <c r="C3" s="65"/>
+      <c r="D3" s="65"/>
+      <c r="E3" s="65"/>
+      <c r="F3" s="65"/>
+      <c r="G3" s="65"/>
+      <c r="H3" s="65"/>
       <c r="I3" s="32" t="s">
         <v>41</v>
       </c>
@@ -6098,14 +6098,14 @@
       <c r="L3" s="28"/>
     </row>
     <row r="4" spans="1:17" ht="15" customHeight="1">
-      <c r="A4" s="74"/>
-      <c r="B4" s="74"/>
-      <c r="C4" s="74"/>
-      <c r="D4" s="74"/>
-      <c r="E4" s="74"/>
-      <c r="F4" s="74"/>
-      <c r="G4" s="74"/>
-      <c r="H4" s="74"/>
+      <c r="A4" s="65"/>
+      <c r="B4" s="65"/>
+      <c r="C4" s="65"/>
+      <c r="D4" s="65"/>
+      <c r="E4" s="65"/>
+      <c r="F4" s="65"/>
+      <c r="G4" s="65"/>
+      <c r="H4" s="65"/>
       <c r="I4" s="33" t="s">
         <v>40</v>
       </c>
@@ -6120,18 +6120,18 @@
       </c>
     </row>
     <row r="5" spans="1:17" ht="15" customHeight="1">
-      <c r="A5" s="73"/>
-      <c r="B5" s="73"/>
-      <c r="C5" s="73"/>
-      <c r="D5" s="73"/>
-      <c r="E5" s="73"/>
-      <c r="F5" s="73"/>
-      <c r="G5" s="73"/>
-      <c r="H5" s="73"/>
-      <c r="I5" s="73"/>
-      <c r="J5" s="73"/>
-      <c r="K5" s="73"/>
-      <c r="L5" s="73"/>
+      <c r="A5" s="58"/>
+      <c r="B5" s="58"/>
+      <c r="C5" s="58"/>
+      <c r="D5" s="58"/>
+      <c r="E5" s="58"/>
+      <c r="F5" s="58"/>
+      <c r="G5" s="58"/>
+      <c r="H5" s="58"/>
+      <c r="I5" s="58"/>
+      <c r="J5" s="58"/>
+      <c r="K5" s="58"/>
+      <c r="L5" s="58"/>
     </row>
     <row r="6" spans="1:17" s="15" customFormat="1" ht="17.25" customHeight="1">
       <c r="A6" s="36" t="s">
@@ -6149,10 +6149,10 @@
       <c r="E6" s="40" t="s">
         <v>57</v>
       </c>
-      <c r="F6" s="65" t="s">
+      <c r="F6" s="67" t="s">
         <v>58</v>
       </c>
-      <c r="G6" s="66"/>
+      <c r="G6" s="68"/>
       <c r="H6" s="36" t="s">
         <v>15</v>
       </c>
@@ -6185,16 +6185,16 @@
       </c>
     </row>
     <row r="7" spans="1:17" ht="15" customHeight="1">
-      <c r="A7" s="67" t="s">
+      <c r="A7" s="59" t="s">
         <v>143</v>
       </c>
-      <c r="B7" s="56" t="s">
+      <c r="B7" s="61" t="s">
         <v>137</v>
       </c>
-      <c r="C7" s="67" t="s">
+      <c r="C7" s="59" t="s">
         <v>138</v>
       </c>
-      <c r="D7" s="67" t="s">
+      <c r="D7" s="59" t="s">
         <v>141</v>
       </c>
       <c r="E7" s="41" t="s">
@@ -6207,17 +6207,17 @@
       <c r="J7" s="14"/>
       <c r="K7" s="14"/>
       <c r="L7" s="14"/>
-      <c r="M7" s="63"/>
+      <c r="M7" s="66"/>
       <c r="N7" s="14"/>
       <c r="O7" s="14"/>
       <c r="P7" s="14"/>
       <c r="Q7" s="14"/>
     </row>
     <row r="8" spans="1:17">
-      <c r="A8" s="68"/>
-      <c r="B8" s="57"/>
-      <c r="C8" s="68"/>
-      <c r="D8" s="68"/>
+      <c r="A8" s="60"/>
+      <c r="B8" s="62"/>
+      <c r="C8" s="60"/>
+      <c r="D8" s="60"/>
       <c r="E8" s="41" t="s">
         <v>135</v>
       </c>
@@ -6228,17 +6228,17 @@
       <c r="J8" s="13"/>
       <c r="K8" s="14"/>
       <c r="L8" s="14"/>
-      <c r="M8" s="63"/>
+      <c r="M8" s="66"/>
       <c r="N8" s="14"/>
       <c r="O8" s="14"/>
       <c r="P8" s="14"/>
       <c r="Q8" s="14"/>
     </row>
     <row r="9" spans="1:17" ht="21.75" customHeight="1">
-      <c r="A9" s="68"/>
-      <c r="B9" s="58"/>
-      <c r="C9" s="69"/>
-      <c r="D9" s="69"/>
+      <c r="A9" s="60"/>
+      <c r="B9" s="63"/>
+      <c r="C9" s="64"/>
+      <c r="D9" s="64"/>
       <c r="E9" s="41" t="s">
         <v>136</v>
       </c>
@@ -6249,7 +6249,7 @@
       <c r="J9" s="13"/>
       <c r="K9" s="14"/>
       <c r="L9" s="14"/>
-      <c r="M9" s="63"/>
+      <c r="M9" s="66"/>
       <c r="N9" s="14"/>
       <c r="O9" s="14"/>
       <c r="P9" s="14"/>
@@ -6275,16 +6275,16 @@
       <c r="Q10" s="36"/>
     </row>
     <row r="11" spans="1:17">
-      <c r="A11" s="56" t="s">
+      <c r="A11" s="61" t="s">
         <v>113</v>
       </c>
-      <c r="B11" s="56" t="s">
+      <c r="B11" s="61" t="s">
         <v>110</v>
       </c>
-      <c r="C11" s="67" t="s">
+      <c r="C11" s="59" t="s">
         <v>101</v>
       </c>
-      <c r="D11" s="67" t="s">
+      <c r="D11" s="59" t="s">
         <v>96</v>
       </c>
       <c r="E11" s="41" t="s">
@@ -6297,17 +6297,17 @@
       <c r="J11" s="44"/>
       <c r="K11" s="43"/>
       <c r="L11" s="14"/>
-      <c r="M11" s="63"/>
+      <c r="M11" s="66"/>
       <c r="N11" s="14"/>
       <c r="O11" s="14"/>
       <c r="P11" s="14"/>
       <c r="Q11" s="14"/>
     </row>
     <row r="12" spans="1:17" ht="15" customHeight="1">
-      <c r="A12" s="57"/>
-      <c r="B12" s="57"/>
-      <c r="C12" s="68"/>
-      <c r="D12" s="68"/>
+      <c r="A12" s="62"/>
+      <c r="B12" s="62"/>
+      <c r="C12" s="60"/>
+      <c r="D12" s="60"/>
       <c r="E12" s="41" t="s">
         <v>99</v>
       </c>
@@ -6322,17 +6322,17 @@
       <c r="J12" s="45"/>
       <c r="K12" s="45"/>
       <c r="L12" s="14"/>
-      <c r="M12" s="63"/>
+      <c r="M12" s="66"/>
       <c r="N12" s="14"/>
       <c r="O12" s="14"/>
       <c r="P12" s="14"/>
       <c r="Q12" s="14"/>
     </row>
     <row r="13" spans="1:17" ht="15" customHeight="1">
-      <c r="A13" s="57"/>
-      <c r="B13" s="57"/>
-      <c r="C13" s="68"/>
-      <c r="D13" s="68"/>
+      <c r="A13" s="62"/>
+      <c r="B13" s="62"/>
+      <c r="C13" s="60"/>
+      <c r="D13" s="60"/>
       <c r="E13" s="41" t="s">
         <v>97</v>
       </c>
@@ -6347,17 +6347,17 @@
       <c r="J13" s="45"/>
       <c r="K13" s="45"/>
       <c r="L13" s="14"/>
-      <c r="M13" s="63"/>
+      <c r="M13" s="66"/>
       <c r="N13" s="14"/>
       <c r="O13" s="14"/>
       <c r="P13" s="14"/>
       <c r="Q13" s="14"/>
     </row>
-    <row r="14" spans="1:17" ht="20.399999999999999">
-      <c r="A14" s="57"/>
-      <c r="B14" s="57"/>
-      <c r="C14" s="68"/>
-      <c r="D14" s="68"/>
+    <row r="14" spans="1:17" ht="22.5">
+      <c r="A14" s="62"/>
+      <c r="B14" s="62"/>
+      <c r="C14" s="60"/>
+      <c r="D14" s="60"/>
       <c r="E14" s="41" t="s">
         <v>100</v>
       </c>
@@ -6376,17 +6376,17 @@
         <v>107</v>
       </c>
       <c r="L14" s="14"/>
-      <c r="M14" s="63"/>
+      <c r="M14" s="66"/>
       <c r="N14" s="14"/>
       <c r="O14" s="14"/>
       <c r="P14" s="14"/>
       <c r="Q14" s="14"/>
     </row>
     <row r="15" spans="1:17" ht="15" customHeight="1">
-      <c r="A15" s="58"/>
-      <c r="B15" s="58"/>
-      <c r="C15" s="69"/>
-      <c r="D15" s="69"/>
+      <c r="A15" s="63"/>
+      <c r="B15" s="63"/>
+      <c r="C15" s="64"/>
+      <c r="D15" s="64"/>
       <c r="E15" s="41" t="s">
         <v>102</v>
       </c>
@@ -6397,7 +6397,7 @@
       <c r="J15" s="45"/>
       <c r="K15" s="45"/>
       <c r="L15" s="14"/>
-      <c r="M15" s="64"/>
+      <c r="M15" s="72"/>
       <c r="N15" s="14"/>
       <c r="O15" s="14"/>
       <c r="P15" s="14"/>
@@ -6423,16 +6423,16 @@
       <c r="Q16" s="36"/>
     </row>
     <row r="17" spans="1:17">
-      <c r="A17" s="67" t="s">
+      <c r="A17" s="59" t="s">
         <v>144</v>
       </c>
-      <c r="B17" s="56" t="s">
+      <c r="B17" s="61" t="s">
         <v>140</v>
       </c>
-      <c r="C17" s="67" t="s">
+      <c r="C17" s="59" t="s">
         <v>139</v>
       </c>
-      <c r="D17" s="67" t="s">
+      <c r="D17" s="59" t="s">
         <v>142</v>
       </c>
       <c r="E17" s="51" t="s">
@@ -6445,17 +6445,17 @@
       <c r="J17" s="14"/>
       <c r="K17" s="14"/>
       <c r="L17" s="14"/>
-      <c r="M17" s="63"/>
+      <c r="M17" s="66"/>
       <c r="N17" s="14"/>
       <c r="O17" s="14"/>
       <c r="P17" s="14"/>
       <c r="Q17" s="14"/>
     </row>
-    <row r="18" spans="1:17">
-      <c r="A18" s="68"/>
-      <c r="B18" s="57"/>
-      <c r="C18" s="68"/>
-      <c r="D18" s="68"/>
+    <row r="18" spans="1:17" ht="22.5">
+      <c r="A18" s="60"/>
+      <c r="B18" s="62"/>
+      <c r="C18" s="60"/>
+      <c r="D18" s="60"/>
       <c r="E18" s="51" t="s">
         <v>146</v>
       </c>
@@ -6466,18 +6466,18 @@
       <c r="J18" s="13"/>
       <c r="K18" s="14"/>
       <c r="L18" s="14"/>
-      <c r="M18" s="63"/>
+      <c r="M18" s="66"/>
       <c r="N18" s="14"/>
       <c r="O18" s="14"/>
       <c r="P18" s="14"/>
       <c r="Q18" s="14"/>
     </row>
     <row r="19" spans="1:17">
-      <c r="A19" s="68"/>
-      <c r="B19" s="57"/>
-      <c r="C19" s="68"/>
-      <c r="D19" s="68"/>
-      <c r="E19" s="70" t="s">
+      <c r="A19" s="60"/>
+      <c r="B19" s="62"/>
+      <c r="C19" s="60"/>
+      <c r="D19" s="60"/>
+      <c r="E19" s="73" t="s">
         <v>147</v>
       </c>
       <c r="F19" s="39" t="s">
@@ -6491,18 +6491,18 @@
       <c r="J19" s="13"/>
       <c r="K19" s="14"/>
       <c r="L19" s="14"/>
-      <c r="M19" s="63"/>
+      <c r="M19" s="66"/>
       <c r="N19" s="14"/>
       <c r="O19" s="14"/>
       <c r="P19" s="14"/>
       <c r="Q19" s="14"/>
     </row>
     <row r="20" spans="1:17">
-      <c r="A20" s="68"/>
-      <c r="B20" s="57"/>
-      <c r="C20" s="68"/>
-      <c r="D20" s="68"/>
-      <c r="E20" s="70"/>
+      <c r="A20" s="60"/>
+      <c r="B20" s="62"/>
+      <c r="C20" s="60"/>
+      <c r="D20" s="60"/>
+      <c r="E20" s="73"/>
       <c r="F20" s="39" t="s">
         <v>152</v>
       </c>
@@ -6514,18 +6514,18 @@
       <c r="J20" s="13"/>
       <c r="K20" s="14"/>
       <c r="L20" s="14"/>
-      <c r="M20" s="63"/>
+      <c r="M20" s="66"/>
       <c r="N20" s="14"/>
       <c r="O20" s="14"/>
       <c r="P20" s="14"/>
       <c r="Q20" s="14"/>
     </row>
     <row r="21" spans="1:17">
-      <c r="A21" s="68"/>
-      <c r="B21" s="57"/>
-      <c r="C21" s="68"/>
-      <c r="D21" s="68"/>
-      <c r="E21" s="70"/>
+      <c r="A21" s="60"/>
+      <c r="B21" s="62"/>
+      <c r="C21" s="60"/>
+      <c r="D21" s="60"/>
+      <c r="E21" s="73"/>
       <c r="F21" s="39" t="s">
         <v>151</v>
       </c>
@@ -6537,18 +6537,18 @@
       <c r="J21" s="13"/>
       <c r="K21" s="14"/>
       <c r="L21" s="14"/>
-      <c r="M21" s="63"/>
+      <c r="M21" s="66"/>
       <c r="N21" s="14"/>
       <c r="O21" s="14"/>
       <c r="P21" s="14"/>
       <c r="Q21" s="14"/>
     </row>
-    <row r="22" spans="1:17">
-      <c r="A22" s="68"/>
-      <c r="B22" s="57"/>
-      <c r="C22" s="68"/>
-      <c r="D22" s="68"/>
-      <c r="E22" s="70"/>
+    <row r="22" spans="1:17" ht="22.5">
+      <c r="A22" s="60"/>
+      <c r="B22" s="62"/>
+      <c r="C22" s="60"/>
+      <c r="D22" s="60"/>
+      <c r="E22" s="73"/>
       <c r="F22" s="39" t="s">
         <v>153</v>
       </c>
@@ -6560,18 +6560,18 @@
       <c r="J22" s="13"/>
       <c r="K22" s="14"/>
       <c r="L22" s="14"/>
-      <c r="M22" s="63"/>
+      <c r="M22" s="66"/>
       <c r="N22" s="14"/>
       <c r="O22" s="14"/>
       <c r="P22" s="14"/>
       <c r="Q22" s="14"/>
     </row>
     <row r="23" spans="1:17">
-      <c r="A23" s="68"/>
-      <c r="B23" s="57"/>
-      <c r="C23" s="68"/>
-      <c r="D23" s="68"/>
-      <c r="E23" s="70"/>
+      <c r="A23" s="60"/>
+      <c r="B23" s="62"/>
+      <c r="C23" s="60"/>
+      <c r="D23" s="60"/>
+      <c r="E23" s="73"/>
       <c r="F23" s="39" t="s">
         <v>154</v>
       </c>
@@ -6583,18 +6583,18 @@
       <c r="J23" s="13"/>
       <c r="K23" s="14"/>
       <c r="L23" s="14"/>
-      <c r="M23" s="63"/>
+      <c r="M23" s="66"/>
       <c r="N23" s="14"/>
       <c r="O23" s="14"/>
       <c r="P23" s="14"/>
       <c r="Q23" s="14"/>
     </row>
     <row r="24" spans="1:17">
-      <c r="A24" s="68"/>
-      <c r="B24" s="57"/>
-      <c r="C24" s="68"/>
-      <c r="D24" s="68"/>
-      <c r="E24" s="70"/>
+      <c r="A24" s="60"/>
+      <c r="B24" s="62"/>
+      <c r="C24" s="60"/>
+      <c r="D24" s="60"/>
+      <c r="E24" s="73"/>
       <c r="F24" s="39"/>
       <c r="G24" s="39"/>
       <c r="H24" s="14"/>
@@ -6602,17 +6602,17 @@
       <c r="J24" s="13"/>
       <c r="K24" s="14"/>
       <c r="L24" s="14"/>
-      <c r="M24" s="63"/>
+      <c r="M24" s="66"/>
       <c r="N24" s="14"/>
       <c r="O24" s="14"/>
       <c r="P24" s="14"/>
       <c r="Q24" s="14"/>
     </row>
     <row r="25" spans="1:17">
-      <c r="A25" s="68"/>
-      <c r="B25" s="57"/>
-      <c r="C25" s="68"/>
-      <c r="D25" s="68"/>
+      <c r="A25" s="60"/>
+      <c r="B25" s="62"/>
+      <c r="C25" s="60"/>
+      <c r="D25" s="60"/>
       <c r="E25" s="51" t="s">
         <v>148</v>
       </c>
@@ -6623,17 +6623,17 @@
       <c r="J25" s="14"/>
       <c r="K25" s="14"/>
       <c r="L25" s="14"/>
-      <c r="M25" s="63"/>
+      <c r="M25" s="66"/>
       <c r="N25" s="14"/>
       <c r="O25" s="14"/>
       <c r="P25" s="14"/>
       <c r="Q25" s="14"/>
     </row>
     <row r="26" spans="1:17">
-      <c r="A26" s="69"/>
-      <c r="B26" s="58"/>
-      <c r="C26" s="69"/>
-      <c r="D26" s="69"/>
+      <c r="A26" s="64"/>
+      <c r="B26" s="63"/>
+      <c r="C26" s="64"/>
+      <c r="D26" s="64"/>
       <c r="E26" s="51" t="s">
         <v>149</v>
       </c>
@@ -6644,7 +6644,7 @@
       <c r="J26" s="13"/>
       <c r="K26" s="14"/>
       <c r="L26" s="14"/>
-      <c r="M26" s="64"/>
+      <c r="M26" s="72"/>
       <c r="N26" s="14"/>
       <c r="O26" s="14"/>
       <c r="P26" s="14"/>
@@ -6669,17 +6669,17 @@
       <c r="P27" s="36"/>
       <c r="Q27" s="36"/>
     </row>
-    <row r="28" spans="1:17" ht="30.6">
-      <c r="A28" s="67" t="s">
+    <row r="28" spans="1:17" ht="33.75">
+      <c r="A28" s="59" t="s">
         <v>114</v>
       </c>
-      <c r="B28" s="67" t="s">
+      <c r="B28" s="59" t="s">
         <v>111</v>
       </c>
-      <c r="C28" s="67" t="s">
+      <c r="C28" s="59" t="s">
         <v>133</v>
       </c>
-      <c r="D28" s="59" t="s">
+      <c r="D28" s="69" t="s">
         <v>112</v>
       </c>
       <c r="E28" s="51" t="s">
@@ -6691,26 +6691,26 @@
       <c r="I28" s="41"/>
       <c r="J28" s="41"/>
       <c r="K28" s="41"/>
-      <c r="L28" s="59" t="s">
+      <c r="L28" s="69" t="s">
         <v>108</v>
       </c>
-      <c r="M28" s="62" t="s">
+      <c r="M28" s="74" t="s">
         <v>68</v>
       </c>
-      <c r="N28" s="56"/>
-      <c r="O28" s="56"/>
-      <c r="P28" s="56" t="s">
+      <c r="N28" s="61"/>
+      <c r="O28" s="61"/>
+      <c r="P28" s="61" t="s">
         <v>67</v>
       </c>
-      <c r="Q28" s="56" t="s">
+      <c r="Q28" s="61" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="29" spans="1:17" ht="15" customHeight="1">
-      <c r="A29" s="68"/>
-      <c r="B29" s="68"/>
-      <c r="C29" s="68"/>
-      <c r="D29" s="60"/>
+      <c r="A29" s="60"/>
+      <c r="B29" s="60"/>
+      <c r="C29" s="60"/>
+      <c r="D29" s="70"/>
       <c r="E29" s="51" t="s">
         <v>116</v>
       </c>
@@ -6720,18 +6720,18 @@
       <c r="I29" s="41"/>
       <c r="J29" s="41"/>
       <c r="K29" s="41"/>
-      <c r="L29" s="60"/>
-      <c r="M29" s="63"/>
-      <c r="N29" s="57"/>
-      <c r="O29" s="57"/>
-      <c r="P29" s="57"/>
-      <c r="Q29" s="57"/>
-    </row>
-    <row r="30" spans="1:17" ht="20.399999999999999">
-      <c r="A30" s="68"/>
-      <c r="B30" s="68"/>
-      <c r="C30" s="68"/>
-      <c r="D30" s="60"/>
+      <c r="L29" s="70"/>
+      <c r="M29" s="66"/>
+      <c r="N29" s="62"/>
+      <c r="O29" s="62"/>
+      <c r="P29" s="62"/>
+      <c r="Q29" s="62"/>
+    </row>
+    <row r="30" spans="1:17" ht="22.5">
+      <c r="A30" s="60"/>
+      <c r="B30" s="60"/>
+      <c r="C30" s="60"/>
+      <c r="D30" s="70"/>
       <c r="E30" s="51" t="s">
         <v>117</v>
       </c>
@@ -6741,18 +6741,18 @@
       <c r="I30" s="41"/>
       <c r="J30" s="41"/>
       <c r="K30" s="41"/>
-      <c r="L30" s="60"/>
-      <c r="M30" s="63"/>
-      <c r="N30" s="57"/>
-      <c r="O30" s="57"/>
-      <c r="P30" s="57"/>
-      <c r="Q30" s="57"/>
-    </row>
-    <row r="31" spans="1:17" ht="20.399999999999999">
-      <c r="A31" s="68"/>
-      <c r="B31" s="68"/>
-      <c r="C31" s="68"/>
-      <c r="D31" s="60"/>
+      <c r="L30" s="70"/>
+      <c r="M30" s="66"/>
+      <c r="N30" s="62"/>
+      <c r="O30" s="62"/>
+      <c r="P30" s="62"/>
+      <c r="Q30" s="62"/>
+    </row>
+    <row r="31" spans="1:17" ht="22.5">
+      <c r="A31" s="60"/>
+      <c r="B31" s="60"/>
+      <c r="C31" s="60"/>
+      <c r="D31" s="70"/>
       <c r="E31" s="51" t="s">
         <v>118</v>
       </c>
@@ -6762,18 +6762,18 @@
       <c r="I31" s="41"/>
       <c r="J31" s="41"/>
       <c r="K31" s="41"/>
-      <c r="L31" s="60"/>
-      <c r="M31" s="63"/>
-      <c r="N31" s="57"/>
-      <c r="O31" s="57"/>
-      <c r="P31" s="57"/>
-      <c r="Q31" s="57"/>
-    </row>
-    <row r="32" spans="1:17">
-      <c r="A32" s="68"/>
-      <c r="B32" s="68"/>
-      <c r="C32" s="68"/>
-      <c r="D32" s="60"/>
+      <c r="L31" s="70"/>
+      <c r="M31" s="66"/>
+      <c r="N31" s="62"/>
+      <c r="O31" s="62"/>
+      <c r="P31" s="62"/>
+      <c r="Q31" s="62"/>
+    </row>
+    <row r="32" spans="1:17" ht="22.5">
+      <c r="A32" s="60"/>
+      <c r="B32" s="60"/>
+      <c r="C32" s="60"/>
+      <c r="D32" s="70"/>
       <c r="E32" s="51" t="s">
         <v>119</v>
       </c>
@@ -6783,18 +6783,18 @@
       <c r="I32" s="41"/>
       <c r="J32" s="41"/>
       <c r="K32" s="41"/>
-      <c r="L32" s="60"/>
-      <c r="M32" s="63"/>
-      <c r="N32" s="57"/>
-      <c r="O32" s="57"/>
-      <c r="P32" s="57"/>
-      <c r="Q32" s="57"/>
-    </row>
-    <row r="33" spans="1:17" ht="20.399999999999999">
-      <c r="A33" s="68"/>
-      <c r="B33" s="68"/>
-      <c r="C33" s="68"/>
-      <c r="D33" s="60"/>
+      <c r="L32" s="70"/>
+      <c r="M32" s="66"/>
+      <c r="N32" s="62"/>
+      <c r="O32" s="62"/>
+      <c r="P32" s="62"/>
+      <c r="Q32" s="62"/>
+    </row>
+    <row r="33" spans="1:17" ht="22.5">
+      <c r="A33" s="60"/>
+      <c r="B33" s="60"/>
+      <c r="C33" s="60"/>
+      <c r="D33" s="70"/>
       <c r="E33" s="51" t="s">
         <v>120</v>
       </c>
@@ -6804,18 +6804,18 @@
       <c r="I33" s="41"/>
       <c r="J33" s="41"/>
       <c r="K33" s="41"/>
-      <c r="L33" s="60"/>
-      <c r="M33" s="63"/>
-      <c r="N33" s="57"/>
-      <c r="O33" s="57"/>
-      <c r="P33" s="57"/>
-      <c r="Q33" s="57"/>
+      <c r="L33" s="70"/>
+      <c r="M33" s="66"/>
+      <c r="N33" s="62"/>
+      <c r="O33" s="62"/>
+      <c r="P33" s="62"/>
+      <c r="Q33" s="62"/>
     </row>
     <row r="34" spans="1:17">
-      <c r="A34" s="68"/>
-      <c r="B34" s="68"/>
-      <c r="C34" s="68"/>
-      <c r="D34" s="60"/>
+      <c r="A34" s="60"/>
+      <c r="B34" s="60"/>
+      <c r="C34" s="60"/>
+      <c r="D34" s="70"/>
       <c r="E34" s="51" t="s">
         <v>121</v>
       </c>
@@ -6825,18 +6825,18 @@
       <c r="I34" s="41"/>
       <c r="J34" s="41"/>
       <c r="K34" s="41"/>
-      <c r="L34" s="60"/>
-      <c r="M34" s="63"/>
-      <c r="N34" s="57"/>
-      <c r="O34" s="57"/>
-      <c r="P34" s="57"/>
-      <c r="Q34" s="57"/>
+      <c r="L34" s="70"/>
+      <c r="M34" s="66"/>
+      <c r="N34" s="62"/>
+      <c r="O34" s="62"/>
+      <c r="P34" s="62"/>
+      <c r="Q34" s="62"/>
     </row>
     <row r="35" spans="1:17">
-      <c r="A35" s="68"/>
-      <c r="B35" s="68"/>
-      <c r="C35" s="68"/>
-      <c r="D35" s="60"/>
+      <c r="A35" s="60"/>
+      <c r="B35" s="60"/>
+      <c r="C35" s="60"/>
+      <c r="D35" s="70"/>
       <c r="E35" s="51" t="s">
         <v>122</v>
       </c>
@@ -6846,18 +6846,18 @@
       <c r="I35" s="41"/>
       <c r="J35" s="41"/>
       <c r="K35" s="41"/>
-      <c r="L35" s="60"/>
-      <c r="M35" s="63"/>
-      <c r="N35" s="57"/>
-      <c r="O35" s="57"/>
-      <c r="P35" s="57"/>
-      <c r="Q35" s="57"/>
-    </row>
-    <row r="36" spans="1:17">
-      <c r="A36" s="68"/>
-      <c r="B36" s="68"/>
-      <c r="C36" s="68"/>
-      <c r="D36" s="60"/>
+      <c r="L35" s="70"/>
+      <c r="M35" s="66"/>
+      <c r="N35" s="62"/>
+      <c r="O35" s="62"/>
+      <c r="P35" s="62"/>
+      <c r="Q35" s="62"/>
+    </row>
+    <row r="36" spans="1:17" ht="22.5">
+      <c r="A36" s="60"/>
+      <c r="B36" s="60"/>
+      <c r="C36" s="60"/>
+      <c r="D36" s="70"/>
       <c r="E36" s="51" t="s">
         <v>127</v>
       </c>
@@ -6867,18 +6867,18 @@
       <c r="I36" s="41"/>
       <c r="J36" s="41"/>
       <c r="K36" s="41"/>
-      <c r="L36" s="60"/>
-      <c r="M36" s="63"/>
-      <c r="N36" s="57"/>
-      <c r="O36" s="57"/>
-      <c r="P36" s="57"/>
-      <c r="Q36" s="57"/>
+      <c r="L36" s="70"/>
+      <c r="M36" s="66"/>
+      <c r="N36" s="62"/>
+      <c r="O36" s="62"/>
+      <c r="P36" s="62"/>
+      <c r="Q36" s="62"/>
     </row>
     <row r="37" spans="1:17">
-      <c r="A37" s="68"/>
-      <c r="B37" s="68"/>
-      <c r="C37" s="68"/>
-      <c r="D37" s="60"/>
+      <c r="A37" s="60"/>
+      <c r="B37" s="60"/>
+      <c r="C37" s="60"/>
+      <c r="D37" s="70"/>
       <c r="E37" s="51" t="s">
         <v>123</v>
       </c>
@@ -6888,18 +6888,18 @@
       <c r="I37" s="41"/>
       <c r="J37" s="41"/>
       <c r="K37" s="41"/>
-      <c r="L37" s="60"/>
-      <c r="M37" s="63"/>
-      <c r="N37" s="57"/>
-      <c r="O37" s="57"/>
-      <c r="P37" s="57"/>
-      <c r="Q37" s="57"/>
-    </row>
-    <row r="38" spans="1:17" ht="20.399999999999999">
-      <c r="A38" s="68"/>
-      <c r="B38" s="68"/>
-      <c r="C38" s="68"/>
-      <c r="D38" s="60"/>
+      <c r="L37" s="70"/>
+      <c r="M37" s="66"/>
+      <c r="N37" s="62"/>
+      <c r="O37" s="62"/>
+      <c r="P37" s="62"/>
+      <c r="Q37" s="62"/>
+    </row>
+    <row r="38" spans="1:17" ht="22.5">
+      <c r="A38" s="60"/>
+      <c r="B38" s="60"/>
+      <c r="C38" s="60"/>
+      <c r="D38" s="70"/>
       <c r="E38" s="51" t="s">
         <v>128</v>
       </c>
@@ -6909,18 +6909,18 @@
       <c r="I38" s="41"/>
       <c r="J38" s="41"/>
       <c r="K38" s="41"/>
-      <c r="L38" s="60"/>
-      <c r="M38" s="63"/>
-      <c r="N38" s="57"/>
-      <c r="O38" s="57"/>
-      <c r="P38" s="57"/>
-      <c r="Q38" s="57"/>
+      <c r="L38" s="70"/>
+      <c r="M38" s="66"/>
+      <c r="N38" s="62"/>
+      <c r="O38" s="62"/>
+      <c r="P38" s="62"/>
+      <c r="Q38" s="62"/>
     </row>
     <row r="39" spans="1:17">
-      <c r="A39" s="68"/>
-      <c r="B39" s="68"/>
-      <c r="C39" s="68"/>
-      <c r="D39" s="60"/>
+      <c r="A39" s="60"/>
+      <c r="B39" s="60"/>
+      <c r="C39" s="60"/>
+      <c r="D39" s="70"/>
       <c r="E39" s="51" t="s">
         <v>124</v>
       </c>
@@ -6930,18 +6930,18 @@
       <c r="I39" s="41"/>
       <c r="J39" s="41"/>
       <c r="K39" s="41"/>
-      <c r="L39" s="60"/>
-      <c r="M39" s="63"/>
-      <c r="N39" s="57"/>
-      <c r="O39" s="57"/>
-      <c r="P39" s="57"/>
-      <c r="Q39" s="57"/>
-    </row>
-    <row r="40" spans="1:17">
-      <c r="A40" s="68"/>
-      <c r="B40" s="68"/>
-      <c r="C40" s="68"/>
-      <c r="D40" s="60"/>
+      <c r="L39" s="70"/>
+      <c r="M39" s="66"/>
+      <c r="N39" s="62"/>
+      <c r="O39" s="62"/>
+      <c r="P39" s="62"/>
+      <c r="Q39" s="62"/>
+    </row>
+    <row r="40" spans="1:17" ht="22.5">
+      <c r="A40" s="60"/>
+      <c r="B40" s="60"/>
+      <c r="C40" s="60"/>
+      <c r="D40" s="70"/>
       <c r="E40" s="51" t="s">
         <v>129</v>
       </c>
@@ -6951,18 +6951,18 @@
       <c r="I40" s="41"/>
       <c r="J40" s="41"/>
       <c r="K40" s="41"/>
-      <c r="L40" s="60"/>
-      <c r="M40" s="63"/>
-      <c r="N40" s="57"/>
-      <c r="O40" s="57"/>
-      <c r="P40" s="57"/>
-      <c r="Q40" s="57"/>
-    </row>
-    <row r="41" spans="1:17" ht="20.399999999999999">
-      <c r="A41" s="68"/>
-      <c r="B41" s="68"/>
-      <c r="C41" s="68"/>
-      <c r="D41" s="60"/>
+      <c r="L40" s="70"/>
+      <c r="M40" s="66"/>
+      <c r="N40" s="62"/>
+      <c r="O40" s="62"/>
+      <c r="P40" s="62"/>
+      <c r="Q40" s="62"/>
+    </row>
+    <row r="41" spans="1:17" ht="22.5">
+      <c r="A41" s="60"/>
+      <c r="B41" s="60"/>
+      <c r="C41" s="60"/>
+      <c r="D41" s="70"/>
       <c r="E41" s="51" t="s">
         <v>125</v>
       </c>
@@ -6972,18 +6972,18 @@
       <c r="I41" s="41"/>
       <c r="J41" s="41"/>
       <c r="K41" s="41"/>
-      <c r="L41" s="60"/>
-      <c r="M41" s="63"/>
-      <c r="N41" s="57"/>
-      <c r="O41" s="57"/>
-      <c r="P41" s="57"/>
-      <c r="Q41" s="57"/>
+      <c r="L41" s="70"/>
+      <c r="M41" s="66"/>
+      <c r="N41" s="62"/>
+      <c r="O41" s="62"/>
+      <c r="P41" s="62"/>
+      <c r="Q41" s="62"/>
     </row>
     <row r="42" spans="1:17">
-      <c r="A42" s="68"/>
-      <c r="B42" s="68"/>
-      <c r="C42" s="68"/>
-      <c r="D42" s="60"/>
+      <c r="A42" s="60"/>
+      <c r="B42" s="60"/>
+      <c r="C42" s="60"/>
+      <c r="D42" s="70"/>
       <c r="E42" s="51" t="s">
         <v>130</v>
       </c>
@@ -6993,18 +6993,18 @@
       <c r="I42" s="41"/>
       <c r="J42" s="41"/>
       <c r="K42" s="41"/>
-      <c r="L42" s="60"/>
-      <c r="M42" s="63"/>
-      <c r="N42" s="57"/>
-      <c r="O42" s="57"/>
-      <c r="P42" s="57"/>
-      <c r="Q42" s="57"/>
-    </row>
-    <row r="43" spans="1:17" ht="20.399999999999999">
-      <c r="A43" s="68"/>
-      <c r="B43" s="68"/>
-      <c r="C43" s="68"/>
-      <c r="D43" s="60"/>
+      <c r="L42" s="70"/>
+      <c r="M42" s="66"/>
+      <c r="N42" s="62"/>
+      <c r="O42" s="62"/>
+      <c r="P42" s="62"/>
+      <c r="Q42" s="62"/>
+    </row>
+    <row r="43" spans="1:17" ht="22.5">
+      <c r="A43" s="60"/>
+      <c r="B43" s="60"/>
+      <c r="C43" s="60"/>
+      <c r="D43" s="70"/>
       <c r="E43" s="51" t="s">
         <v>126</v>
       </c>
@@ -7014,18 +7014,18 @@
       <c r="I43" s="41"/>
       <c r="J43" s="41"/>
       <c r="K43" s="41"/>
-      <c r="L43" s="60"/>
-      <c r="M43" s="63"/>
-      <c r="N43" s="57"/>
-      <c r="O43" s="57"/>
-      <c r="P43" s="57"/>
-      <c r="Q43" s="57"/>
+      <c r="L43" s="70"/>
+      <c r="M43" s="66"/>
+      <c r="N43" s="62"/>
+      <c r="O43" s="62"/>
+      <c r="P43" s="62"/>
+      <c r="Q43" s="62"/>
     </row>
     <row r="44" spans="1:17">
-      <c r="A44" s="68"/>
-      <c r="B44" s="68"/>
-      <c r="C44" s="68"/>
-      <c r="D44" s="60"/>
+      <c r="A44" s="60"/>
+      <c r="B44" s="60"/>
+      <c r="C44" s="60"/>
+      <c r="D44" s="70"/>
       <c r="E44" s="51" t="s">
         <v>131</v>
       </c>
@@ -7035,18 +7035,18 @@
       <c r="I44" s="41"/>
       <c r="J44" s="41"/>
       <c r="K44" s="41"/>
-      <c r="L44" s="60"/>
-      <c r="M44" s="63"/>
-      <c r="N44" s="57"/>
-      <c r="O44" s="57"/>
-      <c r="P44" s="57"/>
-      <c r="Q44" s="57"/>
+      <c r="L44" s="70"/>
+      <c r="M44" s="66"/>
+      <c r="N44" s="62"/>
+      <c r="O44" s="62"/>
+      <c r="P44" s="62"/>
+      <c r="Q44" s="62"/>
     </row>
     <row r="45" spans="1:17" ht="15" customHeight="1">
-      <c r="A45" s="68"/>
-      <c r="B45" s="68"/>
-      <c r="C45" s="68"/>
-      <c r="D45" s="61"/>
+      <c r="A45" s="60"/>
+      <c r="B45" s="60"/>
+      <c r="C45" s="60"/>
+      <c r="D45" s="71"/>
       <c r="E45" s="51" t="s">
         <v>132</v>
       </c>
@@ -7056,12 +7056,12 @@
       <c r="I45" s="41"/>
       <c r="J45" s="41"/>
       <c r="K45" s="41"/>
-      <c r="L45" s="61"/>
-      <c r="M45" s="64"/>
-      <c r="N45" s="58"/>
-      <c r="O45" s="58"/>
-      <c r="P45" s="58"/>
-      <c r="Q45" s="58"/>
+      <c r="L45" s="71"/>
+      <c r="M45" s="72"/>
+      <c r="N45" s="63"/>
+      <c r="O45" s="63"/>
+      <c r="P45" s="63"/>
+      <c r="Q45" s="63"/>
     </row>
     <row r="46" spans="1:17">
       <c r="A46" s="36"/>
@@ -7084,17 +7084,12 @@
     </row>
   </sheetData>
   <mergeCells count="30">
-    <mergeCell ref="A1:H1"/>
-    <mergeCell ref="A5:L5"/>
-    <mergeCell ref="A7:A9"/>
-    <mergeCell ref="A11:A15"/>
-    <mergeCell ref="B11:B15"/>
-    <mergeCell ref="C11:C15"/>
-    <mergeCell ref="D11:D15"/>
-    <mergeCell ref="A2:H4"/>
-    <mergeCell ref="B7:B9"/>
-    <mergeCell ref="C7:C9"/>
-    <mergeCell ref="D7:D9"/>
+    <mergeCell ref="O28:O45"/>
+    <mergeCell ref="P28:P45"/>
+    <mergeCell ref="Q28:Q45"/>
+    <mergeCell ref="L28:L45"/>
+    <mergeCell ref="N28:N45"/>
+    <mergeCell ref="M28:M45"/>
     <mergeCell ref="M7:M9"/>
     <mergeCell ref="F6:G6"/>
     <mergeCell ref="D28:D45"/>
@@ -7108,12 +7103,17 @@
     <mergeCell ref="A17:A26"/>
     <mergeCell ref="C17:C26"/>
     <mergeCell ref="E19:E24"/>
-    <mergeCell ref="O28:O45"/>
-    <mergeCell ref="P28:P45"/>
-    <mergeCell ref="Q28:Q45"/>
-    <mergeCell ref="L28:L45"/>
-    <mergeCell ref="N28:N45"/>
-    <mergeCell ref="M28:M45"/>
+    <mergeCell ref="A1:H1"/>
+    <mergeCell ref="A5:L5"/>
+    <mergeCell ref="A7:A9"/>
+    <mergeCell ref="A11:A15"/>
+    <mergeCell ref="B11:B15"/>
+    <mergeCell ref="C11:C15"/>
+    <mergeCell ref="D11:D15"/>
+    <mergeCell ref="A2:H4"/>
+    <mergeCell ref="B7:B9"/>
+    <mergeCell ref="C7:C9"/>
+    <mergeCell ref="D7:D9"/>
   </mergeCells>
   <conditionalFormatting sqref="A6:B6 H6 F6">
     <cfRule type="containsText" dxfId="109" priority="146" operator="containsText" text="PENDING">
@@ -7497,20 +7497,20 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11:D12"/>
+      <selection activeCell="I19" sqref="I19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="10.199999999999999"/>
+  <sheetFormatPr defaultColWidth="8.75" defaultRowHeight="11.25"/>
   <cols>
-    <col min="1" max="1" width="7.59765625" style="54" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.19921875" style="54" customWidth="1"/>
+    <col min="1" max="1" width="7.625" style="54" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.25" style="54" customWidth="1"/>
     <col min="3" max="3" width="11" style="54" customWidth="1"/>
     <col min="4" max="4" width="14" style="54" customWidth="1"/>
-    <col min="5" max="5" width="12.09765625" style="54" customWidth="1"/>
-    <col min="6" max="16384" width="8.796875" style="54"/>
+    <col min="5" max="5" width="12.125" style="54" customWidth="1"/>
+    <col min="6" max="16384" width="8.75" style="54"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -7545,6 +7545,23 @@
       </c>
       <c r="E2" s="53">
         <v>70000</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3" s="53">
+        <v>30</v>
+      </c>
+      <c r="B3" s="53">
+        <v>30000</v>
+      </c>
+      <c r="C3" s="53">
+        <v>6000</v>
+      </c>
+      <c r="D3" s="53">
+        <v>7000</v>
+      </c>
+      <c r="E3" s="53">
+        <v>80000</v>
       </c>
     </row>
   </sheetData>
@@ -7565,25 +7582,25 @@
       <selection activeCell="C49" sqref="C49"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="1" width="20.59765625" customWidth="1"/>
+    <col min="1" max="1" width="20.625" customWidth="1"/>
     <col min="2" max="2" width="1.5" customWidth="1"/>
-    <col min="3" max="3" width="16.3984375" customWidth="1"/>
-    <col min="4" max="11" width="10.3984375" customWidth="1"/>
-    <col min="16" max="16" width="11.3984375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.375" customWidth="1"/>
+    <col min="4" max="11" width="10.375" customWidth="1"/>
+    <col min="16" max="16" width="11.375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" ht="9.9" customHeight="1">
-      <c r="A1" s="99">
+    <row r="1" spans="1:23" ht="9.9499999999999993" customHeight="1">
+      <c r="A1" s="75">
         <v>41334</v>
       </c>
     </row>
-    <row r="2" spans="1:23" ht="9.9" customHeight="1">
-      <c r="A2" s="100"/>
-    </row>
-    <row r="3" spans="1:23" ht="36.6">
-      <c r="A3" s="100"/>
+    <row r="2" spans="1:23" ht="9.9499999999999993" customHeight="1">
+      <c r="A2" s="76"/>
+    </row>
+    <row r="3" spans="1:23" ht="36.75">
+      <c r="A3" s="76"/>
       <c r="C3" s="1" t="s">
         <v>73</v>
       </c>
@@ -7597,7 +7614,7 @@
       <c r="K3" s="1"/>
     </row>
     <row r="4" spans="1:23" ht="15">
-      <c r="A4" s="101" t="s">
+      <c r="A4" s="77" t="s">
         <v>4</v>
       </c>
       <c r="C4" s="2" t="s">
@@ -7605,132 +7622,132 @@
       </c>
     </row>
     <row r="5" spans="1:23">
-      <c r="A5" s="102"/>
+      <c r="A5" s="78"/>
     </row>
     <row r="6" spans="1:23" ht="14.25" customHeight="1">
-      <c r="A6" s="99">
+      <c r="A6" s="75">
         <v>41485</v>
       </c>
     </row>
     <row r="7" spans="1:23" ht="14.25" customHeight="1">
-      <c r="A7" s="100"/>
+      <c r="A7" s="76"/>
     </row>
     <row r="8" spans="1:23" ht="14.25" customHeight="1">
-      <c r="A8" s="100"/>
-      <c r="C8" s="82" t="s">
+      <c r="A8" s="76"/>
+      <c r="C8" s="85" t="s">
         <v>70</v>
       </c>
-      <c r="D8" s="82"/>
-      <c r="E8" s="82"/>
-      <c r="F8" s="82"/>
-      <c r="G8" s="82"/>
-      <c r="H8" s="82"/>
-      <c r="I8" s="82"/>
-      <c r="J8" s="82"/>
-      <c r="K8" s="82"/>
-      <c r="M8" s="93" t="s">
+      <c r="D8" s="85"/>
+      <c r="E8" s="85"/>
+      <c r="F8" s="85"/>
+      <c r="G8" s="85"/>
+      <c r="H8" s="85"/>
+      <c r="I8" s="85"/>
+      <c r="J8" s="85"/>
+      <c r="K8" s="85"/>
+      <c r="M8" s="96" t="s">
         <v>71</v>
       </c>
-      <c r="N8" s="93"/>
-      <c r="O8" s="93"/>
-      <c r="P8" s="93"/>
-      <c r="Q8" s="93"/>
-      <c r="R8" s="93"/>
-      <c r="S8" s="93"/>
-      <c r="T8" s="93"/>
-      <c r="U8" s="93"/>
-      <c r="V8" s="93"/>
-      <c r="W8" s="93"/>
+      <c r="N8" s="96"/>
+      <c r="O8" s="96"/>
+      <c r="P8" s="96"/>
+      <c r="Q8" s="96"/>
+      <c r="R8" s="96"/>
+      <c r="S8" s="96"/>
+      <c r="T8" s="96"/>
+      <c r="U8" s="96"/>
+      <c r="V8" s="96"/>
+      <c r="W8" s="96"/>
     </row>
     <row r="9" spans="1:23" ht="14.25" customHeight="1">
-      <c r="A9" s="100"/>
-      <c r="C9" s="82"/>
-      <c r="D9" s="82"/>
-      <c r="E9" s="82"/>
-      <c r="F9" s="82"/>
-      <c r="G9" s="82"/>
-      <c r="H9" s="82"/>
-      <c r="I9" s="82"/>
-      <c r="J9" s="82"/>
-      <c r="K9" s="82"/>
-      <c r="M9" s="94"/>
-      <c r="N9" s="94"/>
-      <c r="O9" s="94"/>
-      <c r="P9" s="94"/>
-      <c r="Q9" s="94"/>
-      <c r="R9" s="94"/>
-      <c r="S9" s="94"/>
-      <c r="T9" s="94"/>
-      <c r="U9" s="94"/>
-      <c r="V9" s="94"/>
-      <c r="W9" s="94"/>
+      <c r="A9" s="76"/>
+      <c r="C9" s="85"/>
+      <c r="D9" s="85"/>
+      <c r="E9" s="85"/>
+      <c r="F9" s="85"/>
+      <c r="G9" s="85"/>
+      <c r="H9" s="85"/>
+      <c r="I9" s="85"/>
+      <c r="J9" s="85"/>
+      <c r="K9" s="85"/>
+      <c r="M9" s="97"/>
+      <c r="N9" s="97"/>
+      <c r="O9" s="97"/>
+      <c r="P9" s="97"/>
+      <c r="Q9" s="97"/>
+      <c r="R9" s="97"/>
+      <c r="S9" s="97"/>
+      <c r="T9" s="97"/>
+      <c r="U9" s="97"/>
+      <c r="V9" s="97"/>
+      <c r="W9" s="97"/>
     </row>
     <row r="10" spans="1:23">
-      <c r="A10" s="101" t="s">
+      <c r="A10" s="77" t="s">
         <v>5</v>
       </c>
-      <c r="M10" s="90" t="s">
+      <c r="M10" s="93" t="s">
         <v>80</v>
       </c>
-      <c r="N10" s="91"/>
-      <c r="O10" s="92"/>
-      <c r="P10" s="90" t="s">
+      <c r="N10" s="94"/>
+      <c r="O10" s="95"/>
+      <c r="P10" s="93" t="s">
         <v>75</v>
       </c>
-      <c r="Q10" s="91"/>
-      <c r="R10" s="91"/>
-      <c r="S10" s="91"/>
-      <c r="T10" s="91"/>
-      <c r="U10" s="91"/>
-      <c r="V10" s="91"/>
-      <c r="W10" s="92"/>
+      <c r="Q10" s="94"/>
+      <c r="R10" s="94"/>
+      <c r="S10" s="94"/>
+      <c r="T10" s="94"/>
+      <c r="U10" s="94"/>
+      <c r="V10" s="94"/>
+      <c r="W10" s="95"/>
     </row>
     <row r="11" spans="1:23">
-      <c r="A11" s="102"/>
+      <c r="A11" s="78"/>
       <c r="M11" s="37"/>
       <c r="N11" s="37"/>
       <c r="O11" s="37"/>
-      <c r="P11" s="83" t="s">
+      <c r="P11" s="86" t="s">
         <v>78</v>
       </c>
-      <c r="Q11" s="84"/>
-      <c r="R11" s="83" t="s">
+      <c r="Q11" s="87"/>
+      <c r="R11" s="86" t="s">
         <v>81</v>
       </c>
-      <c r="S11" s="84"/>
-      <c r="T11" s="83" t="s">
+      <c r="S11" s="87"/>
+      <c r="T11" s="86" t="s">
         <v>83</v>
       </c>
-      <c r="U11" s="84"/>
-      <c r="V11" s="95" t="s">
+      <c r="U11" s="87"/>
+      <c r="V11" s="98" t="s">
         <v>72</v>
       </c>
-      <c r="W11" s="96"/>
+      <c r="W11" s="99"/>
     </row>
     <row r="12" spans="1:23" ht="14.25" customHeight="1">
-      <c r="A12" s="105">
+      <c r="A12" s="83">
         <v>220</v>
       </c>
       <c r="M12" s="37"/>
       <c r="N12" s="37"/>
       <c r="O12" s="37"/>
-      <c r="P12" s="85" t="s">
+      <c r="P12" s="88" t="s">
         <v>79</v>
       </c>
-      <c r="Q12" s="86"/>
-      <c r="R12" s="85" t="s">
+      <c r="Q12" s="89"/>
+      <c r="R12" s="88" t="s">
         <v>82</v>
       </c>
-      <c r="S12" s="86"/>
-      <c r="T12" s="85" t="s">
+      <c r="S12" s="89"/>
+      <c r="T12" s="88" t="s">
         <v>84</v>
       </c>
-      <c r="U12" s="86"/>
-      <c r="V12" s="97"/>
-      <c r="W12" s="98"/>
+      <c r="U12" s="89"/>
+      <c r="V12" s="100"/>
+      <c r="W12" s="101"/>
     </row>
     <row r="13" spans="1:23" ht="14.25" customHeight="1">
-      <c r="A13" s="106"/>
+      <c r="A13" s="84"/>
       <c r="M13" s="37"/>
       <c r="N13" s="37"/>
       <c r="O13" s="37"/>
@@ -7756,11 +7773,11 @@
       <c r="W13" s="37"/>
     </row>
     <row r="14" spans="1:23" ht="14.25" customHeight="1">
-      <c r="A14" s="106"/>
-      <c r="M14" s="87" t="s">
+      <c r="A14" s="84"/>
+      <c r="M14" s="90" t="s">
         <v>77</v>
       </c>
-      <c r="N14" s="87" t="s">
+      <c r="N14" s="90" t="s">
         <v>90</v>
       </c>
       <c r="O14" s="38" t="s">
@@ -7788,9 +7805,9 @@
       <c r="W14" s="37"/>
     </row>
     <row r="15" spans="1:23" ht="14.25" customHeight="1">
-      <c r="A15" s="106"/>
-      <c r="M15" s="88"/>
-      <c r="N15" s="88"/>
+      <c r="A15" s="84"/>
+      <c r="M15" s="91"/>
+      <c r="N15" s="91"/>
       <c r="O15" s="38" t="s">
         <v>88</v>
       </c>
@@ -7816,11 +7833,11 @@
       <c r="W15" s="37"/>
     </row>
     <row r="16" spans="1:23">
-      <c r="A16" s="103" t="s">
+      <c r="A16" s="79" t="s">
         <v>91</v>
       </c>
-      <c r="M16" s="89"/>
-      <c r="N16" s="89"/>
+      <c r="M16" s="92"/>
+      <c r="N16" s="92"/>
       <c r="O16" s="38" t="s">
         <v>89</v>
       </c>
@@ -7846,7 +7863,7 @@
       <c r="W16" s="37"/>
     </row>
     <row r="17" spans="1:23">
-      <c r="A17" s="104"/>
+      <c r="A17" s="80"/>
       <c r="M17" s="37"/>
       <c r="N17" s="37"/>
       <c r="O17" s="37"/>
@@ -7860,7 +7877,7 @@
       <c r="W17" s="37"/>
     </row>
     <row r="18" spans="1:23" ht="14.25" customHeight="1">
-      <c r="A18" s="105">
+      <c r="A18" s="83">
         <v>180</v>
       </c>
       <c r="M18" s="37"/>
@@ -7876,7 +7893,7 @@
       <c r="W18" s="37"/>
     </row>
     <row r="19" spans="1:23" ht="14.25" customHeight="1">
-      <c r="A19" s="106"/>
+      <c r="A19" s="84"/>
       <c r="M19" s="37"/>
       <c r="N19" s="37"/>
       <c r="O19" s="37"/>
@@ -7890,18 +7907,18 @@
       <c r="W19" s="37"/>
     </row>
     <row r="20" spans="1:23" ht="14.25" customHeight="1">
-      <c r="A20" s="106"/>
-      <c r="C20" s="79" t="s">
+      <c r="A20" s="84"/>
+      <c r="C20" s="104" t="s">
         <v>69</v>
       </c>
-      <c r="D20" s="79"/>
-      <c r="E20" s="79"/>
-      <c r="F20" s="79"/>
-      <c r="G20" s="79"/>
-      <c r="H20" s="79"/>
-      <c r="I20" s="79"/>
-      <c r="J20" s="79"/>
-      <c r="K20" s="79"/>
+      <c r="D20" s="104"/>
+      <c r="E20" s="104"/>
+      <c r="F20" s="104"/>
+      <c r="G20" s="104"/>
+      <c r="H20" s="104"/>
+      <c r="I20" s="104"/>
+      <c r="J20" s="104"/>
+      <c r="K20" s="104"/>
       <c r="M20" s="37"/>
       <c r="N20" s="37"/>
       <c r="O20" s="37"/>
@@ -7915,16 +7932,16 @@
       <c r="W20" s="37"/>
     </row>
     <row r="21" spans="1:23" ht="14.25" customHeight="1">
-      <c r="A21" s="106"/>
-      <c r="C21" s="79"/>
-      <c r="D21" s="79"/>
-      <c r="E21" s="79"/>
-      <c r="F21" s="79"/>
-      <c r="G21" s="79"/>
-      <c r="H21" s="79"/>
-      <c r="I21" s="79"/>
-      <c r="J21" s="79"/>
-      <c r="K21" s="79"/>
+      <c r="A21" s="84"/>
+      <c r="C21" s="104"/>
+      <c r="D21" s="104"/>
+      <c r="E21" s="104"/>
+      <c r="F21" s="104"/>
+      <c r="G21" s="104"/>
+      <c r="H21" s="104"/>
+      <c r="I21" s="104"/>
+      <c r="J21" s="104"/>
+      <c r="K21" s="104"/>
       <c r="M21" s="37"/>
       <c r="N21" s="37"/>
       <c r="O21" s="37"/>
@@ -7938,7 +7955,7 @@
       <c r="W21" s="37"/>
     </row>
     <row r="22" spans="1:23">
-      <c r="A22" s="103" t="s">
+      <c r="A22" s="79" t="s">
         <v>92</v>
       </c>
       <c r="M22" s="37"/>
@@ -7954,7 +7971,7 @@
       <c r="W22" s="37"/>
     </row>
     <row r="23" spans="1:23">
-      <c r="A23" s="104"/>
+      <c r="A23" s="80"/>
       <c r="M23" s="37"/>
       <c r="N23" s="37"/>
       <c r="O23" s="37"/>
@@ -7968,7 +7985,7 @@
       <c r="W23" s="37"/>
     </row>
     <row r="24" spans="1:23" ht="14.25" customHeight="1">
-      <c r="A24" s="80">
+      <c r="A24" s="105">
         <f>StartWeight-EndWeight</f>
         <v>40</v>
       </c>
@@ -7985,7 +8002,7 @@
       <c r="W24" s="37"/>
     </row>
     <row r="25" spans="1:23" ht="14.25" customHeight="1">
-      <c r="A25" s="81"/>
+      <c r="A25" s="106"/>
       <c r="M25" s="37"/>
       <c r="N25" s="37"/>
       <c r="O25" s="37"/>
@@ -7999,7 +8016,7 @@
       <c r="W25" s="37"/>
     </row>
     <row r="26" spans="1:23" ht="14.25" customHeight="1">
-      <c r="A26" s="81"/>
+      <c r="A26" s="106"/>
       <c r="M26" s="37"/>
       <c r="N26" s="37"/>
       <c r="O26" s="37"/>
@@ -8013,7 +8030,7 @@
       <c r="W26" s="37"/>
     </row>
     <row r="27" spans="1:23" ht="14.25" customHeight="1">
-      <c r="A27" s="81"/>
+      <c r="A27" s="106"/>
       <c r="M27" s="37"/>
       <c r="N27" s="37"/>
       <c r="O27" s="37"/>
@@ -8027,7 +8044,7 @@
       <c r="W27" s="37"/>
     </row>
     <row r="28" spans="1:23">
-      <c r="A28" s="77" t="s">
+      <c r="A28" s="81" t="s">
         <v>93</v>
       </c>
       <c r="M28" s="37"/>
@@ -8043,7 +8060,7 @@
       <c r="W28" s="37"/>
     </row>
     <row r="29" spans="1:23">
-      <c r="A29" s="78"/>
+      <c r="A29" s="82"/>
       <c r="J29" s="3"/>
       <c r="K29" s="3"/>
       <c r="M29" s="37"/>
@@ -8059,7 +8076,7 @@
       <c r="W29" s="37"/>
     </row>
     <row r="30" spans="1:23" ht="14.25" customHeight="1">
-      <c r="A30" s="80">
+      <c r="A30" s="105">
         <f>EndDate-StartDate</f>
         <v>151</v>
       </c>
@@ -8078,7 +8095,7 @@
       <c r="W30" s="37"/>
     </row>
     <row r="31" spans="1:23" ht="14.25" customHeight="1">
-      <c r="A31" s="81"/>
+      <c r="A31" s="106"/>
       <c r="J31" s="3"/>
       <c r="K31" s="3"/>
       <c r="M31" s="37"/>
@@ -8094,7 +8111,7 @@
       <c r="W31" s="37"/>
     </row>
     <row r="32" spans="1:23" ht="14.25" customHeight="1">
-      <c r="A32" s="81"/>
+      <c r="A32" s="106"/>
       <c r="J32" s="3"/>
       <c r="K32" s="3"/>
       <c r="M32" s="37"/>
@@ -8110,7 +8127,7 @@
       <c r="W32" s="37"/>
     </row>
     <row r="33" spans="1:23" ht="14.25" customHeight="1">
-      <c r="A33" s="81"/>
+      <c r="A33" s="106"/>
       <c r="J33" s="3"/>
       <c r="K33" s="3"/>
       <c r="M33" s="37"/>
@@ -8126,7 +8143,7 @@
       <c r="W33" s="37"/>
     </row>
     <row r="34" spans="1:23">
-      <c r="A34" s="77" t="s">
+      <c r="A34" s="81" t="s">
         <v>94</v>
       </c>
       <c r="J34" s="3"/>
@@ -8144,7 +8161,7 @@
       <c r="W34" s="37"/>
     </row>
     <row r="35" spans="1:23">
-      <c r="A35" s="78"/>
+      <c r="A35" s="82"/>
       <c r="J35" s="3"/>
       <c r="K35" s="3"/>
       <c r="M35" s="37"/>
@@ -8160,7 +8177,7 @@
       <c r="W35" s="37"/>
     </row>
     <row r="36" spans="1:23" ht="14.25" customHeight="1">
-      <c r="A36" s="75">
+      <c r="A36" s="102">
         <f>WeightGoal/A30</f>
         <v>0.26490066225165565</v>
       </c>
@@ -8179,7 +8196,7 @@
       <c r="W36" s="37"/>
     </row>
     <row r="37" spans="1:23" ht="14.25" customHeight="1">
-      <c r="A37" s="76"/>
+      <c r="A37" s="103"/>
       <c r="C37" s="5"/>
       <c r="D37" s="5"/>
       <c r="E37" s="5"/>
@@ -8202,7 +8219,7 @@
       <c r="W37" s="37"/>
     </row>
     <row r="38" spans="1:23" ht="14.25" customHeight="1">
-      <c r="A38" s="76"/>
+      <c r="A38" s="103"/>
       <c r="M38" s="37"/>
       <c r="N38" s="37"/>
       <c r="O38" s="37"/>
@@ -8216,7 +8233,7 @@
       <c r="W38" s="37"/>
     </row>
     <row r="39" spans="1:23" ht="14.25" customHeight="1">
-      <c r="A39" s="76"/>
+      <c r="A39" s="103"/>
       <c r="M39" s="37"/>
       <c r="N39" s="37"/>
       <c r="O39" s="37"/>
@@ -8230,7 +8247,7 @@
       <c r="W39" s="37"/>
     </row>
     <row r="40" spans="1:23">
-      <c r="A40" s="77" t="s">
+      <c r="A40" s="81" t="s">
         <v>95</v>
       </c>
       <c r="M40" s="37"/>
@@ -8246,7 +8263,7 @@
       <c r="W40" s="37"/>
     </row>
     <row r="41" spans="1:23">
-      <c r="A41" s="78"/>
+      <c r="A41" s="82"/>
       <c r="M41" s="37"/>
       <c r="N41" s="37"/>
       <c r="O41" s="37"/>
@@ -8261,16 +8278,11 @@
     </row>
   </sheetData>
   <mergeCells count="28">
-    <mergeCell ref="A1:A3"/>
-    <mergeCell ref="A4:A5"/>
-    <mergeCell ref="A22:A23"/>
-    <mergeCell ref="A28:A29"/>
-    <mergeCell ref="A34:A35"/>
-    <mergeCell ref="A6:A9"/>
-    <mergeCell ref="A10:A11"/>
-    <mergeCell ref="A16:A17"/>
-    <mergeCell ref="A12:A15"/>
-    <mergeCell ref="A18:A21"/>
+    <mergeCell ref="A36:A39"/>
+    <mergeCell ref="A40:A41"/>
+    <mergeCell ref="C20:K21"/>
+    <mergeCell ref="A24:A27"/>
+    <mergeCell ref="A30:A33"/>
     <mergeCell ref="C8:K9"/>
     <mergeCell ref="R11:S11"/>
     <mergeCell ref="R12:S12"/>
@@ -8284,11 +8296,16 @@
     <mergeCell ref="T11:U11"/>
     <mergeCell ref="T12:U12"/>
     <mergeCell ref="V11:W12"/>
-    <mergeCell ref="A36:A39"/>
-    <mergeCell ref="A40:A41"/>
-    <mergeCell ref="C20:K21"/>
-    <mergeCell ref="A24:A27"/>
-    <mergeCell ref="A30:A33"/>
+    <mergeCell ref="A1:A3"/>
+    <mergeCell ref="A4:A5"/>
+    <mergeCell ref="A22:A23"/>
+    <mergeCell ref="A28:A29"/>
+    <mergeCell ref="A34:A35"/>
+    <mergeCell ref="A6:A9"/>
+    <mergeCell ref="A10:A11"/>
+    <mergeCell ref="A16:A17"/>
+    <mergeCell ref="A12:A15"/>
+    <mergeCell ref="A18:A21"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.4" right="0.4" top="0.4" bottom="0.4" header="0.3" footer="0.3"/>
@@ -8305,7 +8322,7 @@
       <selection activeCell="H17" sqref="H17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -8320,22 +8337,22 @@
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.8"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="1" width="1.59765625" style="6" customWidth="1"/>
-    <col min="2" max="2" width="12.19921875" style="6" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="2.8984375" style="6" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.59765625" style="6" customWidth="1"/>
-    <col min="5" max="5" width="4.59765625" style="6" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="16.09765625" style="6" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="19.19921875" style="6" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="18.09765625" style="6" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.3984375" style="6" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="4.8984375" style="6" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="1.625" style="6" customWidth="1"/>
+    <col min="2" max="2" width="12.25" style="6" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="2.875" style="6" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.625" style="6" customWidth="1"/>
+    <col min="5" max="5" width="4.625" style="6" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.125" style="6" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="19.25" style="6" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="18.125" style="6" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.375" style="6" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="4.875" style="6" bestFit="1" customWidth="1"/>
     <col min="11" max="16384" width="9" style="6"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:10" ht="36.6">
+    <row r="2" spans="2:10" ht="36.75">
       <c r="B2" s="107" t="s">
         <v>12</v>
       </c>
@@ -8348,7 +8365,7 @@
       <c r="I2" s="107"/>
       <c r="J2" s="107"/>
     </row>
-    <row r="4" spans="2:10">
+    <row r="4" spans="2:10" ht="15">
       <c r="B4" s="11" t="s">
         <v>1</v>
       </c>
@@ -8817,7 +8834,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="20" spans="2:10" ht="36.6">
+    <row r="20" spans="2:10" ht="36.75">
       <c r="B20" s="107" t="s">
         <v>13</v>
       </c>
@@ -8830,7 +8847,7 @@
       <c r="I20" s="107"/>
       <c r="J20" s="107"/>
     </row>
-    <row r="22" spans="2:10">
+    <row r="22" spans="2:10" ht="15">
       <c r="B22" s="11" t="s">
         <v>1</v>
       </c>

</xml_diff>

<commit_message>
tests can now run as per the amount of data provided
</commit_message>
<xml_diff>
--- a/docs/testResources/MasterTestSuite.xlsx
+++ b/docs/testResources/MasterTestSuite.xlsx
@@ -98,7 +98,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="157">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="160">
   <si>
     <t>Last diet entry</t>
   </si>
@@ -570,6 +570,15 @@
   </si>
   <si>
     <t>Password</t>
+  </si>
+  <si>
+    <t>Expected Results</t>
+  </si>
+  <si>
+    <t>R 5,610.61</t>
+  </si>
+  <si>
+    <t>R 7,492.00</t>
   </si>
 </sst>
 </file>
@@ -1067,7 +1076,7 @@
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="108">
+  <cellXfs count="109">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1226,6 +1235,51 @@
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="5" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
+    <xf numFmtId="164" fontId="22" fillId="8" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="22" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="22" fillId="8" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="22" fillId="8" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="22" fillId="8" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="22" fillId="8" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="16" fontId="20" fillId="9" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="20" fillId="9" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="20" fillId="9" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="12" fillId="7" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="12" fillId="7" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="22" fillId="8" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="22" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="22" fillId="8" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="22" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -1235,52 +1289,79 @@
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="164" fontId="22" fillId="8" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="22" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="22" fillId="8" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="22" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="22" fillId="8" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="22" fillId="8" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="16" fontId="20" fillId="9" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="6" fillId="5" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="6" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="3">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="3" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="10" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="12" fillId="7" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="10" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="12" fillId="7" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="11" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="22" fillId="8" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="22" fillId="8" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="22" fillId="8" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="16" fontId="20" fillId="9" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="11" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="1" fontId="22" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="16" fontId="20" fillId="9" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="3" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="14" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="14" fontId="5" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1301,85 +1382,16 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
     <xf numFmtId="2" fontId="5" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="2" fontId="5" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="3" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="10" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="10" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="11" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="11" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="3" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="14" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="6" fillId="5" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="6" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="3">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyFill="1"/>
+    <xf numFmtId="1" fontId="22" fillId="11" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="7">
     <cellStyle name="Heading 1" xfId="1" builtinId="16" customBuiltin="1"/>
@@ -2813,11 +2825,11 @@
         </c:dLbls>
         <c:gapWidth val="90"/>
         <c:overlap val="100"/>
-        <c:axId val="217861744"/>
-        <c:axId val="217862528"/>
+        <c:axId val="410582720"/>
+        <c:axId val="211922816"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="217861744"/>
+        <c:axId val="410582720"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2860,7 +2872,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="217862528"/>
+        <c:crossAx val="211922816"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2868,7 +2880,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="217862528"/>
+        <c:axId val="211922816"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2919,7 +2931,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="217861744"/>
+        <c:crossAx val="410582720"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="0.5"/>
@@ -3099,6 +3111,7 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -3229,8 +3242,8 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="90"/>
-        <c:axId val="217863312"/>
-        <c:axId val="217863704"/>
+        <c:axId val="410957976"/>
+        <c:axId val="410958360"/>
       </c:barChart>
       <c:lineChart>
         <c:grouping val="standard"/>
@@ -3420,11 +3433,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="217863312"/>
-        <c:axId val="217863704"/>
+        <c:axId val="410957976"/>
+        <c:axId val="410958360"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="217863312"/>
+        <c:axId val="410957976"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3467,7 +3480,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="217863704"/>
+        <c:crossAx val="410958360"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3475,7 +3488,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="217863704"/>
+        <c:axId val="410958360"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3538,7 +3551,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="217863312"/>
+        <c:crossAx val="410957976"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -6030,16 +6043,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="30" customHeight="1">
-      <c r="A1" s="56" t="s">
+      <c r="A1" s="71" t="s">
         <v>48</v>
       </c>
-      <c r="B1" s="56"/>
-      <c r="C1" s="56"/>
-      <c r="D1" s="56"/>
-      <c r="E1" s="56"/>
-      <c r="F1" s="56"/>
-      <c r="G1" s="56"/>
-      <c r="H1" s="57"/>
+      <c r="B1" s="71"/>
+      <c r="C1" s="71"/>
+      <c r="D1" s="71"/>
+      <c r="E1" s="71"/>
+      <c r="F1" s="71"/>
+      <c r="G1" s="71"/>
+      <c r="H1" s="72"/>
       <c r="I1" s="34" t="s">
         <v>46</v>
       </c>
@@ -6054,16 +6067,16 @@
       </c>
     </row>
     <row r="2" spans="1:17" ht="15" customHeight="1">
-      <c r="A2" s="65" t="s">
+      <c r="A2" s="74" t="s">
         <v>47</v>
       </c>
-      <c r="B2" s="65"/>
-      <c r="C2" s="65"/>
-      <c r="D2" s="65"/>
-      <c r="E2" s="65"/>
-      <c r="F2" s="65"/>
-      <c r="G2" s="65"/>
-      <c r="H2" s="65"/>
+      <c r="B2" s="74"/>
+      <c r="C2" s="74"/>
+      <c r="D2" s="74"/>
+      <c r="E2" s="74"/>
+      <c r="F2" s="74"/>
+      <c r="G2" s="74"/>
+      <c r="H2" s="74"/>
       <c r="I2" s="33" t="s">
         <v>42</v>
       </c>
@@ -6078,14 +6091,14 @@
       </c>
     </row>
     <row r="3" spans="1:17" ht="15" customHeight="1">
-      <c r="A3" s="65"/>
-      <c r="B3" s="65"/>
-      <c r="C3" s="65"/>
-      <c r="D3" s="65"/>
-      <c r="E3" s="65"/>
-      <c r="F3" s="65"/>
-      <c r="G3" s="65"/>
-      <c r="H3" s="65"/>
+      <c r="A3" s="74"/>
+      <c r="B3" s="74"/>
+      <c r="C3" s="74"/>
+      <c r="D3" s="74"/>
+      <c r="E3" s="74"/>
+      <c r="F3" s="74"/>
+      <c r="G3" s="74"/>
+      <c r="H3" s="74"/>
       <c r="I3" s="32" t="s">
         <v>41</v>
       </c>
@@ -6098,14 +6111,14 @@
       <c r="L3" s="28"/>
     </row>
     <row r="4" spans="1:17" ht="15" customHeight="1">
-      <c r="A4" s="65"/>
-      <c r="B4" s="65"/>
-      <c r="C4" s="65"/>
-      <c r="D4" s="65"/>
-      <c r="E4" s="65"/>
-      <c r="F4" s="65"/>
-      <c r="G4" s="65"/>
-      <c r="H4" s="65"/>
+      <c r="A4" s="74"/>
+      <c r="B4" s="74"/>
+      <c r="C4" s="74"/>
+      <c r="D4" s="74"/>
+      <c r="E4" s="74"/>
+      <c r="F4" s="74"/>
+      <c r="G4" s="74"/>
+      <c r="H4" s="74"/>
       <c r="I4" s="33" t="s">
         <v>40</v>
       </c>
@@ -6120,18 +6133,18 @@
       </c>
     </row>
     <row r="5" spans="1:17" ht="15" customHeight="1">
-      <c r="A5" s="58"/>
-      <c r="B5" s="58"/>
-      <c r="C5" s="58"/>
-      <c r="D5" s="58"/>
-      <c r="E5" s="58"/>
-      <c r="F5" s="58"/>
-      <c r="G5" s="58"/>
-      <c r="H5" s="58"/>
-      <c r="I5" s="58"/>
-      <c r="J5" s="58"/>
-      <c r="K5" s="58"/>
-      <c r="L5" s="58"/>
+      <c r="A5" s="73"/>
+      <c r="B5" s="73"/>
+      <c r="C5" s="73"/>
+      <c r="D5" s="73"/>
+      <c r="E5" s="73"/>
+      <c r="F5" s="73"/>
+      <c r="G5" s="73"/>
+      <c r="H5" s="73"/>
+      <c r="I5" s="73"/>
+      <c r="J5" s="73"/>
+      <c r="K5" s="73"/>
+      <c r="L5" s="73"/>
     </row>
     <row r="6" spans="1:17" s="15" customFormat="1" ht="17.25" customHeight="1">
       <c r="A6" s="36" t="s">
@@ -6149,10 +6162,10 @@
       <c r="E6" s="40" t="s">
         <v>57</v>
       </c>
-      <c r="F6" s="67" t="s">
+      <c r="F6" s="65" t="s">
         <v>58</v>
       </c>
-      <c r="G6" s="68"/>
+      <c r="G6" s="66"/>
       <c r="H6" s="36" t="s">
         <v>15</v>
       </c>
@@ -6185,16 +6198,16 @@
       </c>
     </row>
     <row r="7" spans="1:17" ht="15" customHeight="1">
-      <c r="A7" s="59" t="s">
+      <c r="A7" s="67" t="s">
         <v>143</v>
       </c>
-      <c r="B7" s="61" t="s">
+      <c r="B7" s="56" t="s">
         <v>137</v>
       </c>
-      <c r="C7" s="59" t="s">
+      <c r="C7" s="67" t="s">
         <v>138</v>
       </c>
-      <c r="D7" s="59" t="s">
+      <c r="D7" s="67" t="s">
         <v>141</v>
       </c>
       <c r="E7" s="41" t="s">
@@ -6207,17 +6220,17 @@
       <c r="J7" s="14"/>
       <c r="K7" s="14"/>
       <c r="L7" s="14"/>
-      <c r="M7" s="66"/>
+      <c r="M7" s="63"/>
       <c r="N7" s="14"/>
       <c r="O7" s="14"/>
       <c r="P7" s="14"/>
       <c r="Q7" s="14"/>
     </row>
     <row r="8" spans="1:17">
-      <c r="A8" s="60"/>
-      <c r="B8" s="62"/>
-      <c r="C8" s="60"/>
-      <c r="D8" s="60"/>
+      <c r="A8" s="68"/>
+      <c r="B8" s="57"/>
+      <c r="C8" s="68"/>
+      <c r="D8" s="68"/>
       <c r="E8" s="41" t="s">
         <v>135</v>
       </c>
@@ -6228,17 +6241,17 @@
       <c r="J8" s="13"/>
       <c r="K8" s="14"/>
       <c r="L8" s="14"/>
-      <c r="M8" s="66"/>
+      <c r="M8" s="63"/>
       <c r="N8" s="14"/>
       <c r="O8" s="14"/>
       <c r="P8" s="14"/>
       <c r="Q8" s="14"/>
     </row>
     <row r="9" spans="1:17" ht="21.75" customHeight="1">
-      <c r="A9" s="60"/>
-      <c r="B9" s="63"/>
-      <c r="C9" s="64"/>
-      <c r="D9" s="64"/>
+      <c r="A9" s="68"/>
+      <c r="B9" s="58"/>
+      <c r="C9" s="69"/>
+      <c r="D9" s="69"/>
       <c r="E9" s="41" t="s">
         <v>136</v>
       </c>
@@ -6249,7 +6262,7 @@
       <c r="J9" s="13"/>
       <c r="K9" s="14"/>
       <c r="L9" s="14"/>
-      <c r="M9" s="66"/>
+      <c r="M9" s="63"/>
       <c r="N9" s="14"/>
       <c r="O9" s="14"/>
       <c r="P9" s="14"/>
@@ -6275,16 +6288,16 @@
       <c r="Q10" s="36"/>
     </row>
     <row r="11" spans="1:17">
-      <c r="A11" s="61" t="s">
+      <c r="A11" s="56" t="s">
         <v>113</v>
       </c>
-      <c r="B11" s="61" t="s">
+      <c r="B11" s="56" t="s">
         <v>110</v>
       </c>
-      <c r="C11" s="59" t="s">
+      <c r="C11" s="67" t="s">
         <v>101</v>
       </c>
-      <c r="D11" s="59" t="s">
+      <c r="D11" s="67" t="s">
         <v>96</v>
       </c>
       <c r="E11" s="41" t="s">
@@ -6297,17 +6310,17 @@
       <c r="J11" s="44"/>
       <c r="K11" s="43"/>
       <c r="L11" s="14"/>
-      <c r="M11" s="66"/>
+      <c r="M11" s="63"/>
       <c r="N11" s="14"/>
       <c r="O11" s="14"/>
       <c r="P11" s="14"/>
       <c r="Q11" s="14"/>
     </row>
     <row r="12" spans="1:17" ht="15" customHeight="1">
-      <c r="A12" s="62"/>
-      <c r="B12" s="62"/>
-      <c r="C12" s="60"/>
-      <c r="D12" s="60"/>
+      <c r="A12" s="57"/>
+      <c r="B12" s="57"/>
+      <c r="C12" s="68"/>
+      <c r="D12" s="68"/>
       <c r="E12" s="41" t="s">
         <v>99</v>
       </c>
@@ -6322,17 +6335,17 @@
       <c r="J12" s="45"/>
       <c r="K12" s="45"/>
       <c r="L12" s="14"/>
-      <c r="M12" s="66"/>
+      <c r="M12" s="63"/>
       <c r="N12" s="14"/>
       <c r="O12" s="14"/>
       <c r="P12" s="14"/>
       <c r="Q12" s="14"/>
     </row>
     <row r="13" spans="1:17" ht="15" customHeight="1">
-      <c r="A13" s="62"/>
-      <c r="B13" s="62"/>
-      <c r="C13" s="60"/>
-      <c r="D13" s="60"/>
+      <c r="A13" s="57"/>
+      <c r="B13" s="57"/>
+      <c r="C13" s="68"/>
+      <c r="D13" s="68"/>
       <c r="E13" s="41" t="s">
         <v>97</v>
       </c>
@@ -6347,17 +6360,17 @@
       <c r="J13" s="45"/>
       <c r="K13" s="45"/>
       <c r="L13" s="14"/>
-      <c r="M13" s="66"/>
+      <c r="M13" s="63"/>
       <c r="N13" s="14"/>
       <c r="O13" s="14"/>
       <c r="P13" s="14"/>
       <c r="Q13" s="14"/>
     </row>
     <row r="14" spans="1:17" ht="22.5">
-      <c r="A14" s="62"/>
-      <c r="B14" s="62"/>
-      <c r="C14" s="60"/>
-      <c r="D14" s="60"/>
+      <c r="A14" s="57"/>
+      <c r="B14" s="57"/>
+      <c r="C14" s="68"/>
+      <c r="D14" s="68"/>
       <c r="E14" s="41" t="s">
         <v>100</v>
       </c>
@@ -6376,17 +6389,17 @@
         <v>107</v>
       </c>
       <c r="L14" s="14"/>
-      <c r="M14" s="66"/>
+      <c r="M14" s="63"/>
       <c r="N14" s="14"/>
       <c r="O14" s="14"/>
       <c r="P14" s="14"/>
       <c r="Q14" s="14"/>
     </row>
     <row r="15" spans="1:17" ht="15" customHeight="1">
-      <c r="A15" s="63"/>
-      <c r="B15" s="63"/>
-      <c r="C15" s="64"/>
-      <c r="D15" s="64"/>
+      <c r="A15" s="58"/>
+      <c r="B15" s="58"/>
+      <c r="C15" s="69"/>
+      <c r="D15" s="69"/>
       <c r="E15" s="41" t="s">
         <v>102</v>
       </c>
@@ -6397,7 +6410,7 @@
       <c r="J15" s="45"/>
       <c r="K15" s="45"/>
       <c r="L15" s="14"/>
-      <c r="M15" s="72"/>
+      <c r="M15" s="64"/>
       <c r="N15" s="14"/>
       <c r="O15" s="14"/>
       <c r="P15" s="14"/>
@@ -6423,16 +6436,16 @@
       <c r="Q16" s="36"/>
     </row>
     <row r="17" spans="1:17">
-      <c r="A17" s="59" t="s">
+      <c r="A17" s="67" t="s">
         <v>144</v>
       </c>
-      <c r="B17" s="61" t="s">
+      <c r="B17" s="56" t="s">
         <v>140</v>
       </c>
-      <c r="C17" s="59" t="s">
+      <c r="C17" s="67" t="s">
         <v>139</v>
       </c>
-      <c r="D17" s="59" t="s">
+      <c r="D17" s="67" t="s">
         <v>142</v>
       </c>
       <c r="E17" s="51" t="s">
@@ -6445,17 +6458,17 @@
       <c r="J17" s="14"/>
       <c r="K17" s="14"/>
       <c r="L17" s="14"/>
-      <c r="M17" s="66"/>
+      <c r="M17" s="63"/>
       <c r="N17" s="14"/>
       <c r="O17" s="14"/>
       <c r="P17" s="14"/>
       <c r="Q17" s="14"/>
     </row>
     <row r="18" spans="1:17" ht="22.5">
-      <c r="A18" s="60"/>
-      <c r="B18" s="62"/>
-      <c r="C18" s="60"/>
-      <c r="D18" s="60"/>
+      <c r="A18" s="68"/>
+      <c r="B18" s="57"/>
+      <c r="C18" s="68"/>
+      <c r="D18" s="68"/>
       <c r="E18" s="51" t="s">
         <v>146</v>
       </c>
@@ -6466,18 +6479,18 @@
       <c r="J18" s="13"/>
       <c r="K18" s="14"/>
       <c r="L18" s="14"/>
-      <c r="M18" s="66"/>
+      <c r="M18" s="63"/>
       <c r="N18" s="14"/>
       <c r="O18" s="14"/>
       <c r="P18" s="14"/>
       <c r="Q18" s="14"/>
     </row>
     <row r="19" spans="1:17">
-      <c r="A19" s="60"/>
-      <c r="B19" s="62"/>
-      <c r="C19" s="60"/>
-      <c r="D19" s="60"/>
-      <c r="E19" s="73" t="s">
+      <c r="A19" s="68"/>
+      <c r="B19" s="57"/>
+      <c r="C19" s="68"/>
+      <c r="D19" s="68"/>
+      <c r="E19" s="70" t="s">
         <v>147</v>
       </c>
       <c r="F19" s="39" t="s">
@@ -6491,18 +6504,18 @@
       <c r="J19" s="13"/>
       <c r="K19" s="14"/>
       <c r="L19" s="14"/>
-      <c r="M19" s="66"/>
+      <c r="M19" s="63"/>
       <c r="N19" s="14"/>
       <c r="O19" s="14"/>
       <c r="P19" s="14"/>
       <c r="Q19" s="14"/>
     </row>
     <row r="20" spans="1:17">
-      <c r="A20" s="60"/>
-      <c r="B20" s="62"/>
-      <c r="C20" s="60"/>
-      <c r="D20" s="60"/>
-      <c r="E20" s="73"/>
+      <c r="A20" s="68"/>
+      <c r="B20" s="57"/>
+      <c r="C20" s="68"/>
+      <c r="D20" s="68"/>
+      <c r="E20" s="70"/>
       <c r="F20" s="39" t="s">
         <v>152</v>
       </c>
@@ -6514,18 +6527,18 @@
       <c r="J20" s="13"/>
       <c r="K20" s="14"/>
       <c r="L20" s="14"/>
-      <c r="M20" s="66"/>
+      <c r="M20" s="63"/>
       <c r="N20" s="14"/>
       <c r="O20" s="14"/>
       <c r="P20" s="14"/>
       <c r="Q20" s="14"/>
     </row>
     <row r="21" spans="1:17">
-      <c r="A21" s="60"/>
-      <c r="B21" s="62"/>
-      <c r="C21" s="60"/>
-      <c r="D21" s="60"/>
-      <c r="E21" s="73"/>
+      <c r="A21" s="68"/>
+      <c r="B21" s="57"/>
+      <c r="C21" s="68"/>
+      <c r="D21" s="68"/>
+      <c r="E21" s="70"/>
       <c r="F21" s="39" t="s">
         <v>151</v>
       </c>
@@ -6537,18 +6550,18 @@
       <c r="J21" s="13"/>
       <c r="K21" s="14"/>
       <c r="L21" s="14"/>
-      <c r="M21" s="66"/>
+      <c r="M21" s="63"/>
       <c r="N21" s="14"/>
       <c r="O21" s="14"/>
       <c r="P21" s="14"/>
       <c r="Q21" s="14"/>
     </row>
     <row r="22" spans="1:17" ht="22.5">
-      <c r="A22" s="60"/>
-      <c r="B22" s="62"/>
-      <c r="C22" s="60"/>
-      <c r="D22" s="60"/>
-      <c r="E22" s="73"/>
+      <c r="A22" s="68"/>
+      <c r="B22" s="57"/>
+      <c r="C22" s="68"/>
+      <c r="D22" s="68"/>
+      <c r="E22" s="70"/>
       <c r="F22" s="39" t="s">
         <v>153</v>
       </c>
@@ -6560,18 +6573,18 @@
       <c r="J22" s="13"/>
       <c r="K22" s="14"/>
       <c r="L22" s="14"/>
-      <c r="M22" s="66"/>
+      <c r="M22" s="63"/>
       <c r="N22" s="14"/>
       <c r="O22" s="14"/>
       <c r="P22" s="14"/>
       <c r="Q22" s="14"/>
     </row>
     <row r="23" spans="1:17">
-      <c r="A23" s="60"/>
-      <c r="B23" s="62"/>
-      <c r="C23" s="60"/>
-      <c r="D23" s="60"/>
-      <c r="E23" s="73"/>
+      <c r="A23" s="68"/>
+      <c r="B23" s="57"/>
+      <c r="C23" s="68"/>
+      <c r="D23" s="68"/>
+      <c r="E23" s="70"/>
       <c r="F23" s="39" t="s">
         <v>154</v>
       </c>
@@ -6583,18 +6596,18 @@
       <c r="J23" s="13"/>
       <c r="K23" s="14"/>
       <c r="L23" s="14"/>
-      <c r="M23" s="66"/>
+      <c r="M23" s="63"/>
       <c r="N23" s="14"/>
       <c r="O23" s="14"/>
       <c r="P23" s="14"/>
       <c r="Q23" s="14"/>
     </row>
     <row r="24" spans="1:17">
-      <c r="A24" s="60"/>
-      <c r="B24" s="62"/>
-      <c r="C24" s="60"/>
-      <c r="D24" s="60"/>
-      <c r="E24" s="73"/>
+      <c r="A24" s="68"/>
+      <c r="B24" s="57"/>
+      <c r="C24" s="68"/>
+      <c r="D24" s="68"/>
+      <c r="E24" s="70"/>
       <c r="F24" s="39"/>
       <c r="G24" s="39"/>
       <c r="H24" s="14"/>
@@ -6602,17 +6615,17 @@
       <c r="J24" s="13"/>
       <c r="K24" s="14"/>
       <c r="L24" s="14"/>
-      <c r="M24" s="66"/>
+      <c r="M24" s="63"/>
       <c r="N24" s="14"/>
       <c r="O24" s="14"/>
       <c r="P24" s="14"/>
       <c r="Q24" s="14"/>
     </row>
     <row r="25" spans="1:17">
-      <c r="A25" s="60"/>
-      <c r="B25" s="62"/>
-      <c r="C25" s="60"/>
-      <c r="D25" s="60"/>
+      <c r="A25" s="68"/>
+      <c r="B25" s="57"/>
+      <c r="C25" s="68"/>
+      <c r="D25" s="68"/>
       <c r="E25" s="51" t="s">
         <v>148</v>
       </c>
@@ -6623,17 +6636,17 @@
       <c r="J25" s="14"/>
       <c r="K25" s="14"/>
       <c r="L25" s="14"/>
-      <c r="M25" s="66"/>
+      <c r="M25" s="63"/>
       <c r="N25" s="14"/>
       <c r="O25" s="14"/>
       <c r="P25" s="14"/>
       <c r="Q25" s="14"/>
     </row>
     <row r="26" spans="1:17">
-      <c r="A26" s="64"/>
-      <c r="B26" s="63"/>
-      <c r="C26" s="64"/>
-      <c r="D26" s="64"/>
+      <c r="A26" s="69"/>
+      <c r="B26" s="58"/>
+      <c r="C26" s="69"/>
+      <c r="D26" s="69"/>
       <c r="E26" s="51" t="s">
         <v>149</v>
       </c>
@@ -6644,7 +6657,7 @@
       <c r="J26" s="13"/>
       <c r="K26" s="14"/>
       <c r="L26" s="14"/>
-      <c r="M26" s="72"/>
+      <c r="M26" s="64"/>
       <c r="N26" s="14"/>
       <c r="O26" s="14"/>
       <c r="P26" s="14"/>
@@ -6670,16 +6683,16 @@
       <c r="Q27" s="36"/>
     </row>
     <row r="28" spans="1:17" ht="33.75">
-      <c r="A28" s="59" t="s">
+      <c r="A28" s="67" t="s">
         <v>114</v>
       </c>
-      <c r="B28" s="59" t="s">
+      <c r="B28" s="67" t="s">
         <v>111</v>
       </c>
-      <c r="C28" s="59" t="s">
+      <c r="C28" s="67" t="s">
         <v>133</v>
       </c>
-      <c r="D28" s="69" t="s">
+      <c r="D28" s="59" t="s">
         <v>112</v>
       </c>
       <c r="E28" s="51" t="s">
@@ -6691,26 +6704,26 @@
       <c r="I28" s="41"/>
       <c r="J28" s="41"/>
       <c r="K28" s="41"/>
-      <c r="L28" s="69" t="s">
+      <c r="L28" s="59" t="s">
         <v>108</v>
       </c>
-      <c r="M28" s="74" t="s">
+      <c r="M28" s="62" t="s">
         <v>68</v>
       </c>
-      <c r="N28" s="61"/>
-      <c r="O28" s="61"/>
-      <c r="P28" s="61" t="s">
+      <c r="N28" s="56"/>
+      <c r="O28" s="56"/>
+      <c r="P28" s="56" t="s">
         <v>67</v>
       </c>
-      <c r="Q28" s="61" t="s">
+      <c r="Q28" s="56" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="29" spans="1:17" ht="15" customHeight="1">
-      <c r="A29" s="60"/>
-      <c r="B29" s="60"/>
-      <c r="C29" s="60"/>
-      <c r="D29" s="70"/>
+      <c r="A29" s="68"/>
+      <c r="B29" s="68"/>
+      <c r="C29" s="68"/>
+      <c r="D29" s="60"/>
       <c r="E29" s="51" t="s">
         <v>116</v>
       </c>
@@ -6720,18 +6733,18 @@
       <c r="I29" s="41"/>
       <c r="J29" s="41"/>
       <c r="K29" s="41"/>
-      <c r="L29" s="70"/>
-      <c r="M29" s="66"/>
-      <c r="N29" s="62"/>
-      <c r="O29" s="62"/>
-      <c r="P29" s="62"/>
-      <c r="Q29" s="62"/>
+      <c r="L29" s="60"/>
+      <c r="M29" s="63"/>
+      <c r="N29" s="57"/>
+      <c r="O29" s="57"/>
+      <c r="P29" s="57"/>
+      <c r="Q29" s="57"/>
     </row>
     <row r="30" spans="1:17" ht="22.5">
-      <c r="A30" s="60"/>
-      <c r="B30" s="60"/>
-      <c r="C30" s="60"/>
-      <c r="D30" s="70"/>
+      <c r="A30" s="68"/>
+      <c r="B30" s="68"/>
+      <c r="C30" s="68"/>
+      <c r="D30" s="60"/>
       <c r="E30" s="51" t="s">
         <v>117</v>
       </c>
@@ -6741,18 +6754,18 @@
       <c r="I30" s="41"/>
       <c r="J30" s="41"/>
       <c r="K30" s="41"/>
-      <c r="L30" s="70"/>
-      <c r="M30" s="66"/>
-      <c r="N30" s="62"/>
-      <c r="O30" s="62"/>
-      <c r="P30" s="62"/>
-      <c r="Q30" s="62"/>
+      <c r="L30" s="60"/>
+      <c r="M30" s="63"/>
+      <c r="N30" s="57"/>
+      <c r="O30" s="57"/>
+      <c r="P30" s="57"/>
+      <c r="Q30" s="57"/>
     </row>
     <row r="31" spans="1:17" ht="22.5">
-      <c r="A31" s="60"/>
-      <c r="B31" s="60"/>
-      <c r="C31" s="60"/>
-      <c r="D31" s="70"/>
+      <c r="A31" s="68"/>
+      <c r="B31" s="68"/>
+      <c r="C31" s="68"/>
+      <c r="D31" s="60"/>
       <c r="E31" s="51" t="s">
         <v>118</v>
       </c>
@@ -6762,18 +6775,18 @@
       <c r="I31" s="41"/>
       <c r="J31" s="41"/>
       <c r="K31" s="41"/>
-      <c r="L31" s="70"/>
-      <c r="M31" s="66"/>
-      <c r="N31" s="62"/>
-      <c r="O31" s="62"/>
-      <c r="P31" s="62"/>
-      <c r="Q31" s="62"/>
+      <c r="L31" s="60"/>
+      <c r="M31" s="63"/>
+      <c r="N31" s="57"/>
+      <c r="O31" s="57"/>
+      <c r="P31" s="57"/>
+      <c r="Q31" s="57"/>
     </row>
     <row r="32" spans="1:17" ht="22.5">
-      <c r="A32" s="60"/>
-      <c r="B32" s="60"/>
-      <c r="C32" s="60"/>
-      <c r="D32" s="70"/>
+      <c r="A32" s="68"/>
+      <c r="B32" s="68"/>
+      <c r="C32" s="68"/>
+      <c r="D32" s="60"/>
       <c r="E32" s="51" t="s">
         <v>119</v>
       </c>
@@ -6783,18 +6796,18 @@
       <c r="I32" s="41"/>
       <c r="J32" s="41"/>
       <c r="K32" s="41"/>
-      <c r="L32" s="70"/>
-      <c r="M32" s="66"/>
-      <c r="N32" s="62"/>
-      <c r="O32" s="62"/>
-      <c r="P32" s="62"/>
-      <c r="Q32" s="62"/>
+      <c r="L32" s="60"/>
+      <c r="M32" s="63"/>
+      <c r="N32" s="57"/>
+      <c r="O32" s="57"/>
+      <c r="P32" s="57"/>
+      <c r="Q32" s="57"/>
     </row>
     <row r="33" spans="1:17" ht="22.5">
-      <c r="A33" s="60"/>
-      <c r="B33" s="60"/>
-      <c r="C33" s="60"/>
-      <c r="D33" s="70"/>
+      <c r="A33" s="68"/>
+      <c r="B33" s="68"/>
+      <c r="C33" s="68"/>
+      <c r="D33" s="60"/>
       <c r="E33" s="51" t="s">
         <v>120</v>
       </c>
@@ -6804,18 +6817,18 @@
       <c r="I33" s="41"/>
       <c r="J33" s="41"/>
       <c r="K33" s="41"/>
-      <c r="L33" s="70"/>
-      <c r="M33" s="66"/>
-      <c r="N33" s="62"/>
-      <c r="O33" s="62"/>
-      <c r="P33" s="62"/>
-      <c r="Q33" s="62"/>
+      <c r="L33" s="60"/>
+      <c r="M33" s="63"/>
+      <c r="N33" s="57"/>
+      <c r="O33" s="57"/>
+      <c r="P33" s="57"/>
+      <c r="Q33" s="57"/>
     </row>
     <row r="34" spans="1:17">
-      <c r="A34" s="60"/>
-      <c r="B34" s="60"/>
-      <c r="C34" s="60"/>
-      <c r="D34" s="70"/>
+      <c r="A34" s="68"/>
+      <c r="B34" s="68"/>
+      <c r="C34" s="68"/>
+      <c r="D34" s="60"/>
       <c r="E34" s="51" t="s">
         <v>121</v>
       </c>
@@ -6825,18 +6838,18 @@
       <c r="I34" s="41"/>
       <c r="J34" s="41"/>
       <c r="K34" s="41"/>
-      <c r="L34" s="70"/>
-      <c r="M34" s="66"/>
-      <c r="N34" s="62"/>
-      <c r="O34" s="62"/>
-      <c r="P34" s="62"/>
-      <c r="Q34" s="62"/>
+      <c r="L34" s="60"/>
+      <c r="M34" s="63"/>
+      <c r="N34" s="57"/>
+      <c r="O34" s="57"/>
+      <c r="P34" s="57"/>
+      <c r="Q34" s="57"/>
     </row>
     <row r="35" spans="1:17">
-      <c r="A35" s="60"/>
-      <c r="B35" s="60"/>
-      <c r="C35" s="60"/>
-      <c r="D35" s="70"/>
+      <c r="A35" s="68"/>
+      <c r="B35" s="68"/>
+      <c r="C35" s="68"/>
+      <c r="D35" s="60"/>
       <c r="E35" s="51" t="s">
         <v>122</v>
       </c>
@@ -6846,18 +6859,18 @@
       <c r="I35" s="41"/>
       <c r="J35" s="41"/>
       <c r="K35" s="41"/>
-      <c r="L35" s="70"/>
-      <c r="M35" s="66"/>
-      <c r="N35" s="62"/>
-      <c r="O35" s="62"/>
-      <c r="P35" s="62"/>
-      <c r="Q35" s="62"/>
+      <c r="L35" s="60"/>
+      <c r="M35" s="63"/>
+      <c r="N35" s="57"/>
+      <c r="O35" s="57"/>
+      <c r="P35" s="57"/>
+      <c r="Q35" s="57"/>
     </row>
     <row r="36" spans="1:17" ht="22.5">
-      <c r="A36" s="60"/>
-      <c r="B36" s="60"/>
-      <c r="C36" s="60"/>
-      <c r="D36" s="70"/>
+      <c r="A36" s="68"/>
+      <c r="B36" s="68"/>
+      <c r="C36" s="68"/>
+      <c r="D36" s="60"/>
       <c r="E36" s="51" t="s">
         <v>127</v>
       </c>
@@ -6867,18 +6880,18 @@
       <c r="I36" s="41"/>
       <c r="J36" s="41"/>
       <c r="K36" s="41"/>
-      <c r="L36" s="70"/>
-      <c r="M36" s="66"/>
-      <c r="N36" s="62"/>
-      <c r="O36" s="62"/>
-      <c r="P36" s="62"/>
-      <c r="Q36" s="62"/>
+      <c r="L36" s="60"/>
+      <c r="M36" s="63"/>
+      <c r="N36" s="57"/>
+      <c r="O36" s="57"/>
+      <c r="P36" s="57"/>
+      <c r="Q36" s="57"/>
     </row>
     <row r="37" spans="1:17">
-      <c r="A37" s="60"/>
-      <c r="B37" s="60"/>
-      <c r="C37" s="60"/>
-      <c r="D37" s="70"/>
+      <c r="A37" s="68"/>
+      <c r="B37" s="68"/>
+      <c r="C37" s="68"/>
+      <c r="D37" s="60"/>
       <c r="E37" s="51" t="s">
         <v>123</v>
       </c>
@@ -6888,18 +6901,18 @@
       <c r="I37" s="41"/>
       <c r="J37" s="41"/>
       <c r="K37" s="41"/>
-      <c r="L37" s="70"/>
-      <c r="M37" s="66"/>
-      <c r="N37" s="62"/>
-      <c r="O37" s="62"/>
-      <c r="P37" s="62"/>
-      <c r="Q37" s="62"/>
+      <c r="L37" s="60"/>
+      <c r="M37" s="63"/>
+      <c r="N37" s="57"/>
+      <c r="O37" s="57"/>
+      <c r="P37" s="57"/>
+      <c r="Q37" s="57"/>
     </row>
     <row r="38" spans="1:17" ht="22.5">
-      <c r="A38" s="60"/>
-      <c r="B38" s="60"/>
-      <c r="C38" s="60"/>
-      <c r="D38" s="70"/>
+      <c r="A38" s="68"/>
+      <c r="B38" s="68"/>
+      <c r="C38" s="68"/>
+      <c r="D38" s="60"/>
       <c r="E38" s="51" t="s">
         <v>128</v>
       </c>
@@ -6909,18 +6922,18 @@
       <c r="I38" s="41"/>
       <c r="J38" s="41"/>
       <c r="K38" s="41"/>
-      <c r="L38" s="70"/>
-      <c r="M38" s="66"/>
-      <c r="N38" s="62"/>
-      <c r="O38" s="62"/>
-      <c r="P38" s="62"/>
-      <c r="Q38" s="62"/>
+      <c r="L38" s="60"/>
+      <c r="M38" s="63"/>
+      <c r="N38" s="57"/>
+      <c r="O38" s="57"/>
+      <c r="P38" s="57"/>
+      <c r="Q38" s="57"/>
     </row>
     <row r="39" spans="1:17">
-      <c r="A39" s="60"/>
-      <c r="B39" s="60"/>
-      <c r="C39" s="60"/>
-      <c r="D39" s="70"/>
+      <c r="A39" s="68"/>
+      <c r="B39" s="68"/>
+      <c r="C39" s="68"/>
+      <c r="D39" s="60"/>
       <c r="E39" s="51" t="s">
         <v>124</v>
       </c>
@@ -6930,18 +6943,18 @@
       <c r="I39" s="41"/>
       <c r="J39" s="41"/>
       <c r="K39" s="41"/>
-      <c r="L39" s="70"/>
-      <c r="M39" s="66"/>
-      <c r="N39" s="62"/>
-      <c r="O39" s="62"/>
-      <c r="P39" s="62"/>
-      <c r="Q39" s="62"/>
+      <c r="L39" s="60"/>
+      <c r="M39" s="63"/>
+      <c r="N39" s="57"/>
+      <c r="O39" s="57"/>
+      <c r="P39" s="57"/>
+      <c r="Q39" s="57"/>
     </row>
     <row r="40" spans="1:17" ht="22.5">
-      <c r="A40" s="60"/>
-      <c r="B40" s="60"/>
-      <c r="C40" s="60"/>
-      <c r="D40" s="70"/>
+      <c r="A40" s="68"/>
+      <c r="B40" s="68"/>
+      <c r="C40" s="68"/>
+      <c r="D40" s="60"/>
       <c r="E40" s="51" t="s">
         <v>129</v>
       </c>
@@ -6951,18 +6964,18 @@
       <c r="I40" s="41"/>
       <c r="J40" s="41"/>
       <c r="K40" s="41"/>
-      <c r="L40" s="70"/>
-      <c r="M40" s="66"/>
-      <c r="N40" s="62"/>
-      <c r="O40" s="62"/>
-      <c r="P40" s="62"/>
-      <c r="Q40" s="62"/>
+      <c r="L40" s="60"/>
+      <c r="M40" s="63"/>
+      <c r="N40" s="57"/>
+      <c r="O40" s="57"/>
+      <c r="P40" s="57"/>
+      <c r="Q40" s="57"/>
     </row>
     <row r="41" spans="1:17" ht="22.5">
-      <c r="A41" s="60"/>
-      <c r="B41" s="60"/>
-      <c r="C41" s="60"/>
-      <c r="D41" s="70"/>
+      <c r="A41" s="68"/>
+      <c r="B41" s="68"/>
+      <c r="C41" s="68"/>
+      <c r="D41" s="60"/>
       <c r="E41" s="51" t="s">
         <v>125</v>
       </c>
@@ -6972,18 +6985,18 @@
       <c r="I41" s="41"/>
       <c r="J41" s="41"/>
       <c r="K41" s="41"/>
-      <c r="L41" s="70"/>
-      <c r="M41" s="66"/>
-      <c r="N41" s="62"/>
-      <c r="O41" s="62"/>
-      <c r="P41" s="62"/>
-      <c r="Q41" s="62"/>
+      <c r="L41" s="60"/>
+      <c r="M41" s="63"/>
+      <c r="N41" s="57"/>
+      <c r="O41" s="57"/>
+      <c r="P41" s="57"/>
+      <c r="Q41" s="57"/>
     </row>
     <row r="42" spans="1:17">
-      <c r="A42" s="60"/>
-      <c r="B42" s="60"/>
-      <c r="C42" s="60"/>
-      <c r="D42" s="70"/>
+      <c r="A42" s="68"/>
+      <c r="B42" s="68"/>
+      <c r="C42" s="68"/>
+      <c r="D42" s="60"/>
       <c r="E42" s="51" t="s">
         <v>130</v>
       </c>
@@ -6993,18 +7006,18 @@
       <c r="I42" s="41"/>
       <c r="J42" s="41"/>
       <c r="K42" s="41"/>
-      <c r="L42" s="70"/>
-      <c r="M42" s="66"/>
-      <c r="N42" s="62"/>
-      <c r="O42" s="62"/>
-      <c r="P42" s="62"/>
-      <c r="Q42" s="62"/>
+      <c r="L42" s="60"/>
+      <c r="M42" s="63"/>
+      <c r="N42" s="57"/>
+      <c r="O42" s="57"/>
+      <c r="P42" s="57"/>
+      <c r="Q42" s="57"/>
     </row>
     <row r="43" spans="1:17" ht="22.5">
-      <c r="A43" s="60"/>
-      <c r="B43" s="60"/>
-      <c r="C43" s="60"/>
-      <c r="D43" s="70"/>
+      <c r="A43" s="68"/>
+      <c r="B43" s="68"/>
+      <c r="C43" s="68"/>
+      <c r="D43" s="60"/>
       <c r="E43" s="51" t="s">
         <v>126</v>
       </c>
@@ -7014,18 +7027,18 @@
       <c r="I43" s="41"/>
       <c r="J43" s="41"/>
       <c r="K43" s="41"/>
-      <c r="L43" s="70"/>
-      <c r="M43" s="66"/>
-      <c r="N43" s="62"/>
-      <c r="O43" s="62"/>
-      <c r="P43" s="62"/>
-      <c r="Q43" s="62"/>
+      <c r="L43" s="60"/>
+      <c r="M43" s="63"/>
+      <c r="N43" s="57"/>
+      <c r="O43" s="57"/>
+      <c r="P43" s="57"/>
+      <c r="Q43" s="57"/>
     </row>
     <row r="44" spans="1:17">
-      <c r="A44" s="60"/>
-      <c r="B44" s="60"/>
-      <c r="C44" s="60"/>
-      <c r="D44" s="70"/>
+      <c r="A44" s="68"/>
+      <c r="B44" s="68"/>
+      <c r="C44" s="68"/>
+      <c r="D44" s="60"/>
       <c r="E44" s="51" t="s">
         <v>131</v>
       </c>
@@ -7035,18 +7048,18 @@
       <c r="I44" s="41"/>
       <c r="J44" s="41"/>
       <c r="K44" s="41"/>
-      <c r="L44" s="70"/>
-      <c r="M44" s="66"/>
-      <c r="N44" s="62"/>
-      <c r="O44" s="62"/>
-      <c r="P44" s="62"/>
-      <c r="Q44" s="62"/>
+      <c r="L44" s="60"/>
+      <c r="M44" s="63"/>
+      <c r="N44" s="57"/>
+      <c r="O44" s="57"/>
+      <c r="P44" s="57"/>
+      <c r="Q44" s="57"/>
     </row>
     <row r="45" spans="1:17" ht="15" customHeight="1">
-      <c r="A45" s="60"/>
-      <c r="B45" s="60"/>
-      <c r="C45" s="60"/>
-      <c r="D45" s="71"/>
+      <c r="A45" s="68"/>
+      <c r="B45" s="68"/>
+      <c r="C45" s="68"/>
+      <c r="D45" s="61"/>
       <c r="E45" s="51" t="s">
         <v>132</v>
       </c>
@@ -7056,12 +7069,12 @@
       <c r="I45" s="41"/>
       <c r="J45" s="41"/>
       <c r="K45" s="41"/>
-      <c r="L45" s="71"/>
-      <c r="M45" s="72"/>
-      <c r="N45" s="63"/>
-      <c r="O45" s="63"/>
-      <c r="P45" s="63"/>
-      <c r="Q45" s="63"/>
+      <c r="L45" s="61"/>
+      <c r="M45" s="64"/>
+      <c r="N45" s="58"/>
+      <c r="O45" s="58"/>
+      <c r="P45" s="58"/>
+      <c r="Q45" s="58"/>
     </row>
     <row r="46" spans="1:17">
       <c r="A46" s="36"/>
@@ -7084,12 +7097,17 @@
     </row>
   </sheetData>
   <mergeCells count="30">
-    <mergeCell ref="O28:O45"/>
-    <mergeCell ref="P28:P45"/>
-    <mergeCell ref="Q28:Q45"/>
-    <mergeCell ref="L28:L45"/>
-    <mergeCell ref="N28:N45"/>
-    <mergeCell ref="M28:M45"/>
+    <mergeCell ref="A1:H1"/>
+    <mergeCell ref="A5:L5"/>
+    <mergeCell ref="A7:A9"/>
+    <mergeCell ref="A11:A15"/>
+    <mergeCell ref="B11:B15"/>
+    <mergeCell ref="C11:C15"/>
+    <mergeCell ref="D11:D15"/>
+    <mergeCell ref="A2:H4"/>
+    <mergeCell ref="B7:B9"/>
+    <mergeCell ref="C7:C9"/>
+    <mergeCell ref="D7:D9"/>
     <mergeCell ref="M7:M9"/>
     <mergeCell ref="F6:G6"/>
     <mergeCell ref="D28:D45"/>
@@ -7103,17 +7121,12 @@
     <mergeCell ref="A17:A26"/>
     <mergeCell ref="C17:C26"/>
     <mergeCell ref="E19:E24"/>
-    <mergeCell ref="A1:H1"/>
-    <mergeCell ref="A5:L5"/>
-    <mergeCell ref="A7:A9"/>
-    <mergeCell ref="A11:A15"/>
-    <mergeCell ref="B11:B15"/>
-    <mergeCell ref="C11:C15"/>
-    <mergeCell ref="D11:D15"/>
-    <mergeCell ref="A2:H4"/>
-    <mergeCell ref="B7:B9"/>
-    <mergeCell ref="C7:C9"/>
-    <mergeCell ref="D7:D9"/>
+    <mergeCell ref="O28:O45"/>
+    <mergeCell ref="P28:P45"/>
+    <mergeCell ref="Q28:Q45"/>
+    <mergeCell ref="L28:L45"/>
+    <mergeCell ref="N28:N45"/>
+    <mergeCell ref="M28:M45"/>
   </mergeCells>
   <conditionalFormatting sqref="A6:B6 H6 F6">
     <cfRule type="containsText" dxfId="109" priority="146" operator="containsText" text="PENDING">
@@ -7497,10 +7510,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I19" sqref="I19"/>
+      <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.75" defaultRowHeight="11.25"/>
@@ -7510,10 +7523,11 @@
     <col min="3" max="3" width="11" style="54" customWidth="1"/>
     <col min="4" max="4" width="14" style="54" customWidth="1"/>
     <col min="5" max="5" width="12.125" style="54" customWidth="1"/>
-    <col min="6" max="16384" width="8.75" style="54"/>
+    <col min="6" max="6" width="12.5" style="54" customWidth="1"/>
+    <col min="7" max="16384" width="8.75" style="54"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:6">
       <c r="A1" s="52" t="s">
         <v>150</v>
       </c>
@@ -7529,8 +7543,11 @@
       <c r="E1" s="52" t="s">
         <v>154</v>
       </c>
-    </row>
-    <row r="2" spans="1:5">
+      <c r="F1" s="108" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
       <c r="A2" s="53">
         <v>25</v>
       </c>
@@ -7546,8 +7563,11 @@
       <c r="E2" s="53">
         <v>70000</v>
       </c>
-    </row>
-    <row r="3" spans="1:5">
+      <c r="F2" s="53" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
       <c r="A3" s="53">
         <v>30</v>
       </c>
@@ -7562,6 +7582,9 @@
       </c>
       <c r="E3" s="53">
         <v>80000</v>
+      </c>
+      <c r="F3" s="53" t="s">
+        <v>159</v>
       </c>
     </row>
   </sheetData>
@@ -7592,15 +7615,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:23" ht="9.9499999999999993" customHeight="1">
-      <c r="A1" s="75">
+      <c r="A1" s="99">
         <v>41334</v>
       </c>
     </row>
     <row r="2" spans="1:23" ht="9.9499999999999993" customHeight="1">
-      <c r="A2" s="76"/>
+      <c r="A2" s="100"/>
     </row>
     <row r="3" spans="1:23" ht="36.75">
-      <c r="A3" s="76"/>
+      <c r="A3" s="100"/>
       <c r="C3" s="1" t="s">
         <v>73</v>
       </c>
@@ -7614,7 +7637,7 @@
       <c r="K3" s="1"/>
     </row>
     <row r="4" spans="1:23" ht="15">
-      <c r="A4" s="77" t="s">
+      <c r="A4" s="101" t="s">
         <v>4</v>
       </c>
       <c r="C4" s="2" t="s">
@@ -7622,132 +7645,132 @@
       </c>
     </row>
     <row r="5" spans="1:23">
-      <c r="A5" s="78"/>
+      <c r="A5" s="102"/>
     </row>
     <row r="6" spans="1:23" ht="14.25" customHeight="1">
-      <c r="A6" s="75">
+      <c r="A6" s="99">
         <v>41485</v>
       </c>
     </row>
     <row r="7" spans="1:23" ht="14.25" customHeight="1">
-      <c r="A7" s="76"/>
+      <c r="A7" s="100"/>
     </row>
     <row r="8" spans="1:23" ht="14.25" customHeight="1">
-      <c r="A8" s="76"/>
-      <c r="C8" s="85" t="s">
+      <c r="A8" s="100"/>
+      <c r="C8" s="82" t="s">
         <v>70</v>
       </c>
-      <c r="D8" s="85"/>
-      <c r="E8" s="85"/>
-      <c r="F8" s="85"/>
-      <c r="G8" s="85"/>
-      <c r="H8" s="85"/>
-      <c r="I8" s="85"/>
-      <c r="J8" s="85"/>
-      <c r="K8" s="85"/>
-      <c r="M8" s="96" t="s">
+      <c r="D8" s="82"/>
+      <c r="E8" s="82"/>
+      <c r="F8" s="82"/>
+      <c r="G8" s="82"/>
+      <c r="H8" s="82"/>
+      <c r="I8" s="82"/>
+      <c r="J8" s="82"/>
+      <c r="K8" s="82"/>
+      <c r="M8" s="93" t="s">
         <v>71</v>
       </c>
-      <c r="N8" s="96"/>
-      <c r="O8" s="96"/>
-      <c r="P8" s="96"/>
-      <c r="Q8" s="96"/>
-      <c r="R8" s="96"/>
-      <c r="S8" s="96"/>
-      <c r="T8" s="96"/>
-      <c r="U8" s="96"/>
-      <c r="V8" s="96"/>
-      <c r="W8" s="96"/>
+      <c r="N8" s="93"/>
+      <c r="O8" s="93"/>
+      <c r="P8" s="93"/>
+      <c r="Q8" s="93"/>
+      <c r="R8" s="93"/>
+      <c r="S8" s="93"/>
+      <c r="T8" s="93"/>
+      <c r="U8" s="93"/>
+      <c r="V8" s="93"/>
+      <c r="W8" s="93"/>
     </row>
     <row r="9" spans="1:23" ht="14.25" customHeight="1">
-      <c r="A9" s="76"/>
-      <c r="C9" s="85"/>
-      <c r="D9" s="85"/>
-      <c r="E9" s="85"/>
-      <c r="F9" s="85"/>
-      <c r="G9" s="85"/>
-      <c r="H9" s="85"/>
-      <c r="I9" s="85"/>
-      <c r="J9" s="85"/>
-      <c r="K9" s="85"/>
-      <c r="M9" s="97"/>
-      <c r="N9" s="97"/>
-      <c r="O9" s="97"/>
-      <c r="P9" s="97"/>
-      <c r="Q9" s="97"/>
-      <c r="R9" s="97"/>
-      <c r="S9" s="97"/>
-      <c r="T9" s="97"/>
-      <c r="U9" s="97"/>
-      <c r="V9" s="97"/>
-      <c r="W9" s="97"/>
+      <c r="A9" s="100"/>
+      <c r="C9" s="82"/>
+      <c r="D9" s="82"/>
+      <c r="E9" s="82"/>
+      <c r="F9" s="82"/>
+      <c r="G9" s="82"/>
+      <c r="H9" s="82"/>
+      <c r="I9" s="82"/>
+      <c r="J9" s="82"/>
+      <c r="K9" s="82"/>
+      <c r="M9" s="94"/>
+      <c r="N9" s="94"/>
+      <c r="O9" s="94"/>
+      <c r="P9" s="94"/>
+      <c r="Q9" s="94"/>
+      <c r="R9" s="94"/>
+      <c r="S9" s="94"/>
+      <c r="T9" s="94"/>
+      <c r="U9" s="94"/>
+      <c r="V9" s="94"/>
+      <c r="W9" s="94"/>
     </row>
     <row r="10" spans="1:23">
-      <c r="A10" s="77" t="s">
+      <c r="A10" s="101" t="s">
         <v>5</v>
       </c>
-      <c r="M10" s="93" t="s">
+      <c r="M10" s="90" t="s">
         <v>80</v>
       </c>
-      <c r="N10" s="94"/>
-      <c r="O10" s="95"/>
-      <c r="P10" s="93" t="s">
+      <c r="N10" s="91"/>
+      <c r="O10" s="92"/>
+      <c r="P10" s="90" t="s">
         <v>75</v>
       </c>
-      <c r="Q10" s="94"/>
-      <c r="R10" s="94"/>
-      <c r="S10" s="94"/>
-      <c r="T10" s="94"/>
-      <c r="U10" s="94"/>
-      <c r="V10" s="94"/>
-      <c r="W10" s="95"/>
+      <c r="Q10" s="91"/>
+      <c r="R10" s="91"/>
+      <c r="S10" s="91"/>
+      <c r="T10" s="91"/>
+      <c r="U10" s="91"/>
+      <c r="V10" s="91"/>
+      <c r="W10" s="92"/>
     </row>
     <row r="11" spans="1:23">
-      <c r="A11" s="78"/>
+      <c r="A11" s="102"/>
       <c r="M11" s="37"/>
       <c r="N11" s="37"/>
       <c r="O11" s="37"/>
-      <c r="P11" s="86" t="s">
+      <c r="P11" s="83" t="s">
         <v>78</v>
       </c>
-      <c r="Q11" s="87"/>
-      <c r="R11" s="86" t="s">
+      <c r="Q11" s="84"/>
+      <c r="R11" s="83" t="s">
         <v>81</v>
       </c>
-      <c r="S11" s="87"/>
-      <c r="T11" s="86" t="s">
+      <c r="S11" s="84"/>
+      <c r="T11" s="83" t="s">
         <v>83</v>
       </c>
-      <c r="U11" s="87"/>
-      <c r="V11" s="98" t="s">
+      <c r="U11" s="84"/>
+      <c r="V11" s="95" t="s">
         <v>72</v>
       </c>
-      <c r="W11" s="99"/>
+      <c r="W11" s="96"/>
     </row>
     <row r="12" spans="1:23" ht="14.25" customHeight="1">
-      <c r="A12" s="83">
+      <c r="A12" s="105">
         <v>220</v>
       </c>
       <c r="M12" s="37"/>
       <c r="N12" s="37"/>
       <c r="O12" s="37"/>
-      <c r="P12" s="88" t="s">
+      <c r="P12" s="85" t="s">
         <v>79</v>
       </c>
-      <c r="Q12" s="89"/>
-      <c r="R12" s="88" t="s">
+      <c r="Q12" s="86"/>
+      <c r="R12" s="85" t="s">
         <v>82</v>
       </c>
-      <c r="S12" s="89"/>
-      <c r="T12" s="88" t="s">
+      <c r="S12" s="86"/>
+      <c r="T12" s="85" t="s">
         <v>84</v>
       </c>
-      <c r="U12" s="89"/>
-      <c r="V12" s="100"/>
-      <c r="W12" s="101"/>
+      <c r="U12" s="86"/>
+      <c r="V12" s="97"/>
+      <c r="W12" s="98"/>
     </row>
     <row r="13" spans="1:23" ht="14.25" customHeight="1">
-      <c r="A13" s="84"/>
+      <c r="A13" s="106"/>
       <c r="M13" s="37"/>
       <c r="N13" s="37"/>
       <c r="O13" s="37"/>
@@ -7773,11 +7796,11 @@
       <c r="W13" s="37"/>
     </row>
     <row r="14" spans="1:23" ht="14.25" customHeight="1">
-      <c r="A14" s="84"/>
-      <c r="M14" s="90" t="s">
+      <c r="A14" s="106"/>
+      <c r="M14" s="87" t="s">
         <v>77</v>
       </c>
-      <c r="N14" s="90" t="s">
+      <c r="N14" s="87" t="s">
         <v>90</v>
       </c>
       <c r="O14" s="38" t="s">
@@ -7805,9 +7828,9 @@
       <c r="W14" s="37"/>
     </row>
     <row r="15" spans="1:23" ht="14.25" customHeight="1">
-      <c r="A15" s="84"/>
-      <c r="M15" s="91"/>
-      <c r="N15" s="91"/>
+      <c r="A15" s="106"/>
+      <c r="M15" s="88"/>
+      <c r="N15" s="88"/>
       <c r="O15" s="38" t="s">
         <v>88</v>
       </c>
@@ -7833,11 +7856,11 @@
       <c r="W15" s="37"/>
     </row>
     <row r="16" spans="1:23">
-      <c r="A16" s="79" t="s">
+      <c r="A16" s="103" t="s">
         <v>91</v>
       </c>
-      <c r="M16" s="92"/>
-      <c r="N16" s="92"/>
+      <c r="M16" s="89"/>
+      <c r="N16" s="89"/>
       <c r="O16" s="38" t="s">
         <v>89</v>
       </c>
@@ -7863,7 +7886,7 @@
       <c r="W16" s="37"/>
     </row>
     <row r="17" spans="1:23">
-      <c r="A17" s="80"/>
+      <c r="A17" s="104"/>
       <c r="M17" s="37"/>
       <c r="N17" s="37"/>
       <c r="O17" s="37"/>
@@ -7877,7 +7900,7 @@
       <c r="W17" s="37"/>
     </row>
     <row r="18" spans="1:23" ht="14.25" customHeight="1">
-      <c r="A18" s="83">
+      <c r="A18" s="105">
         <v>180</v>
       </c>
       <c r="M18" s="37"/>
@@ -7893,7 +7916,7 @@
       <c r="W18" s="37"/>
     </row>
     <row r="19" spans="1:23" ht="14.25" customHeight="1">
-      <c r="A19" s="84"/>
+      <c r="A19" s="106"/>
       <c r="M19" s="37"/>
       <c r="N19" s="37"/>
       <c r="O19" s="37"/>
@@ -7907,18 +7930,18 @@
       <c r="W19" s="37"/>
     </row>
     <row r="20" spans="1:23" ht="14.25" customHeight="1">
-      <c r="A20" s="84"/>
-      <c r="C20" s="104" t="s">
+      <c r="A20" s="106"/>
+      <c r="C20" s="79" t="s">
         <v>69</v>
       </c>
-      <c r="D20" s="104"/>
-      <c r="E20" s="104"/>
-      <c r="F20" s="104"/>
-      <c r="G20" s="104"/>
-      <c r="H20" s="104"/>
-      <c r="I20" s="104"/>
-      <c r="J20" s="104"/>
-      <c r="K20" s="104"/>
+      <c r="D20" s="79"/>
+      <c r="E20" s="79"/>
+      <c r="F20" s="79"/>
+      <c r="G20" s="79"/>
+      <c r="H20" s="79"/>
+      <c r="I20" s="79"/>
+      <c r="J20" s="79"/>
+      <c r="K20" s="79"/>
       <c r="M20" s="37"/>
       <c r="N20" s="37"/>
       <c r="O20" s="37"/>
@@ -7932,16 +7955,16 @@
       <c r="W20" s="37"/>
     </row>
     <row r="21" spans="1:23" ht="14.25" customHeight="1">
-      <c r="A21" s="84"/>
-      <c r="C21" s="104"/>
-      <c r="D21" s="104"/>
-      <c r="E21" s="104"/>
-      <c r="F21" s="104"/>
-      <c r="G21" s="104"/>
-      <c r="H21" s="104"/>
-      <c r="I21" s="104"/>
-      <c r="J21" s="104"/>
-      <c r="K21" s="104"/>
+      <c r="A21" s="106"/>
+      <c r="C21" s="79"/>
+      <c r="D21" s="79"/>
+      <c r="E21" s="79"/>
+      <c r="F21" s="79"/>
+      <c r="G21" s="79"/>
+      <c r="H21" s="79"/>
+      <c r="I21" s="79"/>
+      <c r="J21" s="79"/>
+      <c r="K21" s="79"/>
       <c r="M21" s="37"/>
       <c r="N21" s="37"/>
       <c r="O21" s="37"/>
@@ -7955,7 +7978,7 @@
       <c r="W21" s="37"/>
     </row>
     <row r="22" spans="1:23">
-      <c r="A22" s="79" t="s">
+      <c r="A22" s="103" t="s">
         <v>92</v>
       </c>
       <c r="M22" s="37"/>
@@ -7971,7 +7994,7 @@
       <c r="W22" s="37"/>
     </row>
     <row r="23" spans="1:23">
-      <c r="A23" s="80"/>
+      <c r="A23" s="104"/>
       <c r="M23" s="37"/>
       <c r="N23" s="37"/>
       <c r="O23" s="37"/>
@@ -7985,7 +8008,7 @@
       <c r="W23" s="37"/>
     </row>
     <row r="24" spans="1:23" ht="14.25" customHeight="1">
-      <c r="A24" s="105">
+      <c r="A24" s="80">
         <f>StartWeight-EndWeight</f>
         <v>40</v>
       </c>
@@ -8002,7 +8025,7 @@
       <c r="W24" s="37"/>
     </row>
     <row r="25" spans="1:23" ht="14.25" customHeight="1">
-      <c r="A25" s="106"/>
+      <c r="A25" s="81"/>
       <c r="M25" s="37"/>
       <c r="N25" s="37"/>
       <c r="O25" s="37"/>
@@ -8016,7 +8039,7 @@
       <c r="W25" s="37"/>
     </row>
     <row r="26" spans="1:23" ht="14.25" customHeight="1">
-      <c r="A26" s="106"/>
+      <c r="A26" s="81"/>
       <c r="M26" s="37"/>
       <c r="N26" s="37"/>
       <c r="O26" s="37"/>
@@ -8030,7 +8053,7 @@
       <c r="W26" s="37"/>
     </row>
     <row r="27" spans="1:23" ht="14.25" customHeight="1">
-      <c r="A27" s="106"/>
+      <c r="A27" s="81"/>
       <c r="M27" s="37"/>
       <c r="N27" s="37"/>
       <c r="O27" s="37"/>
@@ -8044,7 +8067,7 @@
       <c r="W27" s="37"/>
     </row>
     <row r="28" spans="1:23">
-      <c r="A28" s="81" t="s">
+      <c r="A28" s="77" t="s">
         <v>93</v>
       </c>
       <c r="M28" s="37"/>
@@ -8060,7 +8083,7 @@
       <c r="W28" s="37"/>
     </row>
     <row r="29" spans="1:23">
-      <c r="A29" s="82"/>
+      <c r="A29" s="78"/>
       <c r="J29" s="3"/>
       <c r="K29" s="3"/>
       <c r="M29" s="37"/>
@@ -8076,7 +8099,7 @@
       <c r="W29" s="37"/>
     </row>
     <row r="30" spans="1:23" ht="14.25" customHeight="1">
-      <c r="A30" s="105">
+      <c r="A30" s="80">
         <f>EndDate-StartDate</f>
         <v>151</v>
       </c>
@@ -8095,7 +8118,7 @@
       <c r="W30" s="37"/>
     </row>
     <row r="31" spans="1:23" ht="14.25" customHeight="1">
-      <c r="A31" s="106"/>
+      <c r="A31" s="81"/>
       <c r="J31" s="3"/>
       <c r="K31" s="3"/>
       <c r="M31" s="37"/>
@@ -8111,7 +8134,7 @@
       <c r="W31" s="37"/>
     </row>
     <row r="32" spans="1:23" ht="14.25" customHeight="1">
-      <c r="A32" s="106"/>
+      <c r="A32" s="81"/>
       <c r="J32" s="3"/>
       <c r="K32" s="3"/>
       <c r="M32" s="37"/>
@@ -8127,7 +8150,7 @@
       <c r="W32" s="37"/>
     </row>
     <row r="33" spans="1:23" ht="14.25" customHeight="1">
-      <c r="A33" s="106"/>
+      <c r="A33" s="81"/>
       <c r="J33" s="3"/>
       <c r="K33" s="3"/>
       <c r="M33" s="37"/>
@@ -8143,7 +8166,7 @@
       <c r="W33" s="37"/>
     </row>
     <row r="34" spans="1:23">
-      <c r="A34" s="81" t="s">
+      <c r="A34" s="77" t="s">
         <v>94</v>
       </c>
       <c r="J34" s="3"/>
@@ -8161,7 +8184,7 @@
       <c r="W34" s="37"/>
     </row>
     <row r="35" spans="1:23">
-      <c r="A35" s="82"/>
+      <c r="A35" s="78"/>
       <c r="J35" s="3"/>
       <c r="K35" s="3"/>
       <c r="M35" s="37"/>
@@ -8177,7 +8200,7 @@
       <c r="W35" s="37"/>
     </row>
     <row r="36" spans="1:23" ht="14.25" customHeight="1">
-      <c r="A36" s="102">
+      <c r="A36" s="75">
         <f>WeightGoal/A30</f>
         <v>0.26490066225165565</v>
       </c>
@@ -8196,7 +8219,7 @@
       <c r="W36" s="37"/>
     </row>
     <row r="37" spans="1:23" ht="14.25" customHeight="1">
-      <c r="A37" s="103"/>
+      <c r="A37" s="76"/>
       <c r="C37" s="5"/>
       <c r="D37" s="5"/>
       <c r="E37" s="5"/>
@@ -8219,7 +8242,7 @@
       <c r="W37" s="37"/>
     </row>
     <row r="38" spans="1:23" ht="14.25" customHeight="1">
-      <c r="A38" s="103"/>
+      <c r="A38" s="76"/>
       <c r="M38" s="37"/>
       <c r="N38" s="37"/>
       <c r="O38" s="37"/>
@@ -8233,7 +8256,7 @@
       <c r="W38" s="37"/>
     </row>
     <row r="39" spans="1:23" ht="14.25" customHeight="1">
-      <c r="A39" s="103"/>
+      <c r="A39" s="76"/>
       <c r="M39" s="37"/>
       <c r="N39" s="37"/>
       <c r="O39" s="37"/>
@@ -8247,7 +8270,7 @@
       <c r="W39" s="37"/>
     </row>
     <row r="40" spans="1:23">
-      <c r="A40" s="81" t="s">
+      <c r="A40" s="77" t="s">
         <v>95</v>
       </c>
       <c r="M40" s="37"/>
@@ -8263,7 +8286,7 @@
       <c r="W40" s="37"/>
     </row>
     <row r="41" spans="1:23">
-      <c r="A41" s="82"/>
+      <c r="A41" s="78"/>
       <c r="M41" s="37"/>
       <c r="N41" s="37"/>
       <c r="O41" s="37"/>
@@ -8278,11 +8301,16 @@
     </row>
   </sheetData>
   <mergeCells count="28">
-    <mergeCell ref="A36:A39"/>
-    <mergeCell ref="A40:A41"/>
-    <mergeCell ref="C20:K21"/>
-    <mergeCell ref="A24:A27"/>
-    <mergeCell ref="A30:A33"/>
+    <mergeCell ref="A1:A3"/>
+    <mergeCell ref="A4:A5"/>
+    <mergeCell ref="A22:A23"/>
+    <mergeCell ref="A28:A29"/>
+    <mergeCell ref="A34:A35"/>
+    <mergeCell ref="A6:A9"/>
+    <mergeCell ref="A10:A11"/>
+    <mergeCell ref="A16:A17"/>
+    <mergeCell ref="A12:A15"/>
+    <mergeCell ref="A18:A21"/>
     <mergeCell ref="C8:K9"/>
     <mergeCell ref="R11:S11"/>
     <mergeCell ref="R12:S12"/>
@@ -8296,16 +8324,11 @@
     <mergeCell ref="T11:U11"/>
     <mergeCell ref="T12:U12"/>
     <mergeCell ref="V11:W12"/>
-    <mergeCell ref="A1:A3"/>
-    <mergeCell ref="A4:A5"/>
-    <mergeCell ref="A22:A23"/>
-    <mergeCell ref="A28:A29"/>
-    <mergeCell ref="A34:A35"/>
-    <mergeCell ref="A6:A9"/>
-    <mergeCell ref="A10:A11"/>
-    <mergeCell ref="A16:A17"/>
-    <mergeCell ref="A12:A15"/>
-    <mergeCell ref="A18:A21"/>
+    <mergeCell ref="A36:A39"/>
+    <mergeCell ref="A40:A41"/>
+    <mergeCell ref="C20:K21"/>
+    <mergeCell ref="A24:A27"/>
+    <mergeCell ref="A30:A33"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.4" right="0.4" top="0.4" bottom="0.4" header="0.3" footer="0.3"/>

</xml_diff>